<commit_message>
[RF GEN] CPU update-Company
</commit_message>
<xml_diff>
--- a/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
+++ b/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
@@ -1,44 +1,212 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B919A28-5EDA-415C-A879-0753C87C2051}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RFGEN V2.0" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
-  <si>
-    <t>HD1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
   <si>
     <t>+12V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAB1143-04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMA_RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF_OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXD_LCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RXD_LCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIMIT_SW_B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIMIT_SW_A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN_PWM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5267-3P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5267-2P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MX35313-2P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RV_CT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FET_TEMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PW_IS_CT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FW_CT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIAS_ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VDC_IN</t>
+  </si>
+  <si>
+    <t>JP1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP_BIAS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JUMPER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+3.3V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNTRST</t>
+  </si>
+  <si>
+    <t>JTDI</t>
+  </si>
+  <si>
+    <t>SYS_SWDIO</t>
+  </si>
+  <si>
+    <t>SYS_SWCLK</t>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTDO</t>
+  </si>
+  <si>
+    <t>NRST</t>
+  </si>
+  <si>
+    <t>GND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT48V</t>
+  </si>
+  <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LAB1143-04</t>
+    <t>CN104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MX35313-5P</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -46,141 +214,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>J3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMA_RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RF_IN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RF_OUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TH+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TH-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAN1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAN2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXD_LCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RXD_LCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN103</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIMIT_SW_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LIMIT_SW_A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAN_PWM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5267-3P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5267-2P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MX35313-2P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CN100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RV_CT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FET_TEMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PW_IS_CT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FW_CT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BIAS_ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VDC_IN</t>
-  </si>
-  <si>
-    <t>JP1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JP_BIAS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JUMPER</t>
+    <t>RFOUT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMA_ST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5267-8P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN106</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN107</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +280,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -253,51 +326,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -435,18 +463,91 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -456,51 +557,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,18 +610,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -531,6 +655,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -540,25 +667,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>103413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1"/>
+        <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13096875" y="323850"/>
-          <a:ext cx="1333500" cy="371475"/>
+          <a:off x="12268199" y="767442"/>
+          <a:ext cx="1311730" cy="389165"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -605,26 +738,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>737507</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>89806</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2"/>
+        <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5924550" y="342900"/>
-          <a:ext cx="1057275" cy="361950"/>
+          <a:off x="8760278" y="753835"/>
+          <a:ext cx="1515835" cy="508908"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -672,25 +811,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>503465</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>110218</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12392025" y="161925"/>
-          <a:ext cx="3181350" cy="8372475"/>
+          <a:off x="12053208" y="555171"/>
+          <a:ext cx="3687535" cy="10277476"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -733,28 +878,34 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>447676</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
+        <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419726" y="209550"/>
-          <a:ext cx="5476874" cy="9896475"/>
+          <a:off x="5378905" y="533400"/>
+          <a:ext cx="5021034" cy="10809514"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 7008"/>
+            <a:gd name="adj" fmla="val 2056"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -791,32 +942,41 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>524692</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>167369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>153761</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+        <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3476625" y="7639050"/>
-          <a:ext cx="1181100" cy="809625"/>
+          <a:off x="3823063" y="6219826"/>
+          <a:ext cx="1155790" cy="879021"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -841,7 +1001,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -851,7 +1011,7 @@
             </a:rPr>
             <a:t>SMPS</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -863,7 +1023,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -873,7 +1033,7 @@
             </a:rPr>
             <a:t>48V 12.5A</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -885,7 +1045,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -895,7 +1055,7 @@
             </a:rPr>
             <a:t>PSP-600-48</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -910,32 +1070,41 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>530679</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>198664</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9"/>
+        <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11325225" y="6267450"/>
-          <a:ext cx="1162050" cy="809625"/>
+          <a:off x="3829050" y="4718957"/>
+          <a:ext cx="1140279" cy="857250"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
         </a:solidFill>
       </xdr:spPr>
       <xdr:style>
@@ -960,7 +1129,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -970,7 +1139,7 @@
             </a:rPr>
             <a:t>SMPS</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -982,7 +1151,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -992,7 +1161,7 @@
             </a:rPr>
             <a:t>12V 100W</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1007,26 +1176,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>92528</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>575584</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>210910</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6"/>
+        <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7324724" y="4152900"/>
-          <a:ext cx="1381126" cy="695325"/>
+          <a:off x="7222671" y="8229600"/>
+          <a:ext cx="1375684" cy="722539"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1079,26 +1254,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>106135</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>608240</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>189139</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+        <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7305675" y="5153025"/>
-          <a:ext cx="1400175" cy="714375"/>
+          <a:off x="7236278" y="9092292"/>
+          <a:ext cx="1394733" cy="741590"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1152,25 +1333,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>527958</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>91167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:colOff>42183</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10"/>
+        <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3819525" y="5191125"/>
-          <a:ext cx="1162050" cy="809625"/>
+          <a:off x="3826329" y="9964510"/>
+          <a:ext cx="1147083" cy="825953"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1201,7 +1388,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1215,7 +1402,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1225,7 +1412,7 @@
             </a:rPr>
             <a:t>Limit S/W</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1241,25 +1428,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>527958</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>130627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>42183</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>72117</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+        <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3819525" y="4133850"/>
-          <a:ext cx="1162050" cy="819150"/>
+          <a:off x="3826329" y="8871856"/>
+          <a:ext cx="1147083" cy="845004"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1290,7 +1483,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1304,7 +1497,7 @@
         <a:p>
           <a:pPr algn="ctr" rtl="0"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1314,7 +1507,7 @@
             </a:rPr>
             <a:t>Limit S/W</a:t>
           </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1330,25 +1523,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>137433</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>195943</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>613683</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>167368</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="오른쪽 화살표 7"/>
+        <xdr:cNvPr id="8" name="오른쪽 화살표 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5076825" y="4429125"/>
-          <a:ext cx="476250" cy="190500"/>
+          <a:off x="5068662" y="9165772"/>
+          <a:ext cx="476250" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1384,25 +1583,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>127908</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>604158</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>157842</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="오른쪽 화살표 13"/>
+        <xdr:cNvPr id="14" name="오른쪽 화살표 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5067300" y="5495925"/>
-          <a:ext cx="476250" cy="200025"/>
+          <a:off x="5059137" y="10267949"/>
+          <a:ext cx="476250" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1437,26 +1642,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>107495</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>583745</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>110218</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="오른쪽 화살표 14"/>
+        <xdr:cNvPr id="15" name="오른쪽 화살표 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="10782300" y="6591300"/>
-          <a:ext cx="476250" cy="209550"/>
+        <a:xfrm>
+          <a:off x="5038724" y="5029201"/>
+          <a:ext cx="476250" cy="229960"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1499,34 +1710,44 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>141513</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>54430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>617763</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>44905</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
+        <xdr:cNvPr id="16" name="오른쪽 화살표 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E350673-E94C-400E-9271-47D82C523782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1343025" y="352425"/>
-          <a:ext cx="3181350" cy="7143750"/>
+          <a:off x="5072742" y="6553201"/>
+          <a:ext cx="476250" cy="219075"/>
         </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 7008"/>
-          </a:avLst>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19050"/>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1549,9 +1770,165 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
-            <a:noFill/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>530680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>201385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>166004</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDF590CA-A38C-4E79-A6D7-1A694015461B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3829051" y="7603671"/>
+          <a:ext cx="1140279" cy="846362"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Touch LCD</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PC</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>174172</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>642258</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="화살표: 왼쪽/오른쪽 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3004E09F-D64E-44C1-9DA2-F3663D2BA8C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5105401" y="7924800"/>
+          <a:ext cx="468086" cy="174171"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1603,7 +1980,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1636,9 +2013,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1671,6 +2065,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1846,523 +2257,815 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:V37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="I3:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="4.625" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.625" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.625" customWidth="1"/>
-    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
-    <col min="12" max="12" width="5.625" customWidth="1"/>
-    <col min="13" max="13" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.625" customWidth="1"/>
-    <col min="15" max="15" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.59765625" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.59765625" customWidth="1"/>
+    <col min="10" max="10" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.69921875" customWidth="1"/>
+    <col min="13" max="13" width="9.8984375" customWidth="1"/>
+    <col min="14" max="14" width="4.59765625" customWidth="1"/>
+    <col min="15" max="15" width="14.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L4" s="29" t="s">
+    <row r="3" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I6" s="6">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1">
+        <v>6</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I8" s="6">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="1">
+        <v>8</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I9" s="6">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I10" s="6">
+        <v>11</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="1">
+        <v>12</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="36"/>
+    </row>
+    <row r="11" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I11" s="6">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="1">
+        <v>14</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="18"/>
+      <c r="S11" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="T11" s="38"/>
+    </row>
+    <row r="12" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I12" s="6">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="1">
+        <v>16</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" s="2">
+        <v>1</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I13" s="6">
+        <v>17</v>
+      </c>
+      <c r="J13" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="1">
+        <v>18</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="6">
+        <v>2</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="6">
+        <v>2</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I14" s="9">
+        <v>19</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="10">
+        <v>20</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="6">
+        <v>3</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="6">
+        <v>3</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="N15" s="6">
+        <v>4</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" s="6">
+        <v>4</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="N16" s="39">
+        <v>5</v>
+      </c>
+      <c r="O16" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="6">
+        <v>5</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="N17" s="6">
+        <v>6</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17" s="6">
+        <v>6</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="39">
+        <v>7</v>
+      </c>
+      <c r="O18" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="6">
+        <v>7</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I19" s="9">
+        <v>2</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" s="9">
+        <v>8</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="9">
+        <v>8</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="14"/>
+      <c r="N21" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" s="14"/>
+      <c r="S21" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="T21" s="36"/>
+    </row>
+    <row r="22" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="N22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="S22" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="T22" s="38"/>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
-    </row>
-    <row r="5" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="17" t="s">
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="5">
+      <c r="S23" s="2">
+        <v>1</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I24" s="9">
         <v>2</v>
       </c>
-      <c r="O5" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="J24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N24" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="7">
+      <c r="O24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" s="9">
+        <v>2</v>
+      </c>
+      <c r="T24" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="14"/>
+      <c r="N26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" s="14"/>
+      <c r="S26" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="T26" s="22"/>
+    </row>
+    <row r="27" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I27" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="N27" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="O27" s="18"/>
+      <c r="S27" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="T27" s="20"/>
+    </row>
+    <row r="28" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S28" s="2">
+        <v>1</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I29" s="6">
+        <v>2</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N29" s="6">
+        <v>2</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S29" s="6">
+        <v>2</v>
+      </c>
+      <c r="T29" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I30" s="6">
         <v>3</v>
       </c>
-      <c r="N6" s="1">
+      <c r="J30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N30" s="6">
+        <v>3</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S30" s="6">
+        <v>3</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="9:20" x14ac:dyDescent="0.4">
+      <c r="I31" s="6">
         <v>4</v>
       </c>
-      <c r="O6" s="27"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C7" s="7">
+      <c r="J31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N31" s="6">
+        <v>4</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S31" s="6">
+        <v>4</v>
+      </c>
+      <c r="T31" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I32" s="9">
+        <v>5</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="N32" s="9">
+        <v>5</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S32" s="9">
+        <v>5</v>
+      </c>
+      <c r="T32" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="34" spans="9:23" x14ac:dyDescent="0.4">
+      <c r="I34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="14"/>
+      <c r="N34" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O34" s="14"/>
+      <c r="S34" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="T34" s="22"/>
+      <c r="V34" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="W34" s="32"/>
+    </row>
+    <row r="35" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I35" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="18"/>
+      <c r="N35" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="O35" s="30"/>
+      <c r="S35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="T35" s="16"/>
+      <c r="V35" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="W35" s="34"/>
+    </row>
+    <row r="36" spans="9:23" x14ac:dyDescent="0.4">
+      <c r="I36" s="2">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="2">
+        <v>1</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S36" s="2">
+        <v>1</v>
+      </c>
+      <c r="T36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="9:23" x14ac:dyDescent="0.4">
+      <c r="I37" s="6">
+        <v>2</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N37" s="6">
+        <v>2</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S37" s="6">
+        <v>2</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V37" s="6">
+        <v>2</v>
+      </c>
+      <c r="W37" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I38" s="9">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="J38" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="6">
+        <v>3</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S38" s="6">
+        <v>3</v>
+      </c>
+      <c r="T38" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V38" s="6">
+        <v>3</v>
+      </c>
+      <c r="W38" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="N39" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="7">
+      <c r="O39" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S39" s="6">
+        <v>4</v>
+      </c>
+      <c r="T39" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V39" s="6">
+        <v>4</v>
+      </c>
+      <c r="W39" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I40" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="N40" s="9">
         <v>5</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="1">
-        <v>6</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C8" s="7">
+      <c r="O40" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S40" s="9">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="T40" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V40" s="9">
+        <v>5</v>
+      </c>
+      <c r="W40" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I41" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" spans="9:23" x14ac:dyDescent="0.4">
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O42" s="14"/>
+    </row>
+    <row r="43" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I43" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
-        <v>6</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="J43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O43" s="18"/>
+    </row>
+    <row r="44" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="N44" s="2">
+        <v>1</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I45" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45" s="14"/>
+      <c r="N45" s="9">
         <v>2</v>
       </c>
-      <c r="L8" s="7">
-        <v>7</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="1">
-        <v>8</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="7">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="10">
-        <v>9</v>
-      </c>
-      <c r="M9" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="11">
+      <c r="O45" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I46" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="18"/>
+    </row>
+    <row r="47" spans="9:23" x14ac:dyDescent="0.4">
+      <c r="I47" s="2">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N47" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="10">
-        <v>9</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="11">
-        <v>10</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="23"/>
-      <c r="N13" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="23"/>
-      <c r="U13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V13" s="14"/>
-    </row>
-    <row r="14" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I14" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="25"/>
-      <c r="N14" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="25"/>
-      <c r="U14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="V14" s="16"/>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="I15" s="3">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N15" s="3">
-        <v>1</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" s="3">
-        <v>1</v>
-      </c>
-      <c r="V15" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="3:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I16" s="10">
+      <c r="O47" s="14"/>
+    </row>
+    <row r="48" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I48" s="9">
         <v>2</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J48" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O48" s="18"/>
+    </row>
+    <row r="49" spans="11:15" x14ac:dyDescent="0.4">
+      <c r="N49" s="2">
+        <v>1</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="11:15" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="N50" s="9">
+        <v>2</v>
+      </c>
+      <c r="O50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="10">
-        <v>2</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="U16" s="7">
-        <v>2</v>
-      </c>
-      <c r="V16" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="U17" s="7">
-        <v>3</v>
-      </c>
-      <c r="V17" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I18" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="23"/>
-      <c r="N18" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="O18" s="23"/>
-      <c r="U18" s="7">
-        <v>4</v>
-      </c>
-      <c r="V18" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="25"/>
-      <c r="N19" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="25"/>
-      <c r="U19" s="10">
-        <v>5</v>
-      </c>
-      <c r="V19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I20" s="3">
-        <v>1</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N20" s="3">
-        <v>1</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I21" s="10">
-        <v>2</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="10">
-        <v>2</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="U21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="V21" s="14"/>
-    </row>
-    <row r="22" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="U22" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="V22" s="16"/>
-    </row>
-    <row r="23" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I23" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="23"/>
-      <c r="N23" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="O23" s="23"/>
-      <c r="U23" s="3">
-        <v>1</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I24" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="25"/>
-      <c r="N24" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="16"/>
-      <c r="U24" s="7">
-        <v>2</v>
-      </c>
-      <c r="V24" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I25" s="3">
-        <v>1</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25" s="3">
-        <v>1</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U25" s="7">
-        <v>3</v>
-      </c>
-      <c r="V25" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I26" s="7">
-        <v>2</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N26" s="10">
-        <v>2</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="U26" s="7">
-        <v>4</v>
-      </c>
-      <c r="V26" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I27" s="10">
-        <v>3</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="U27" s="10">
-        <v>5</v>
-      </c>
-      <c r="V27" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I29" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="23"/>
-      <c r="U29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="V29" s="14"/>
-    </row>
-    <row r="30" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I30" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="25"/>
-      <c r="U30" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="V30" s="21"/>
-    </row>
-    <row r="31" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I31" s="3">
-        <v>1</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="U31" s="3">
-        <v>1</v>
-      </c>
-      <c r="V31" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="9:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I32" s="10">
-        <v>2</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="U32" s="7">
-        <v>2</v>
-      </c>
-      <c r="V32" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="14:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="U33" s="7">
-        <v>3</v>
-      </c>
-      <c r="V33" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="14:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="O34" s="14"/>
-      <c r="U34" s="10">
-        <v>4</v>
-      </c>
-      <c r="V34" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="14:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N35" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="O35" s="16"/>
-    </row>
-    <row r="36" spans="14:22" x14ac:dyDescent="0.3">
-      <c r="N36" s="3">
-        <v>1</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="14:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N37" s="10">
-        <v>2</v>
-      </c>
-      <c r="O37" s="12" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="59" spans="11:15" x14ac:dyDescent="0.4">
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+    </row>
+    <row r="72" spans="11:12" x14ac:dyDescent="0.4">
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="U22:V22"/>
+  <mergeCells count="35">
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
     <mergeCell ref="N34:O34"/>
     <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="N47:O47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2372,12 +3075,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2385,12 +3088,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[10/27] RF GEN PCB work - home
</commit_message>
<xml_diff>
--- a/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
+++ b/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RFGEN V2.0" sheetId="1" r:id="rId1"/>
     <sheet name="RFGEN V2.0B" sheetId="4" r:id="rId2"/>
     <sheet name="Block1" sheetId="2" r:id="rId3"/>
     <sheet name="Block2" sheetId="5" r:id="rId4"/>
-    <sheet name="Block2 (2)" sheetId="6" r:id="rId5"/>
+    <sheet name="Block3" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -844,39 +844,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -913,6 +882,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,8 +927,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -964,7 +964,7 @@
         <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,7 +1036,7 @@
         <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1108,7 +1108,7 @@
         <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1174,7 +1174,7 @@
         <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1240,7 +1240,7 @@
         <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,7 +1368,7 @@
         <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1474,7 @@
         <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1552,7 +1552,7 @@
         <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1630,7 +1630,7 @@
         <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1725,7 +1725,7 @@
         <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1820,7 +1820,7 @@
         <xdr:cNvPr id="8" name="오른쪽 화살표 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,7 +1880,7 @@
         <xdr:cNvPr id="14" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1940,7 +1940,7 @@
         <xdr:cNvPr id="15" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,7 +2008,7 @@
         <xdr:cNvPr id="16" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2076,7 +2076,7 @@
         <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2174,7 @@
         <xdr:cNvPr id="13" name="화살표: 왼쪽/오른쪽 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2234,7 +2234,7 @@
         <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2315,7 +2315,7 @@
         <xdr:cNvPr id="20" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2383,7 +2383,7 @@
         <xdr:cNvPr id="21" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2451,7 +2451,7 @@
         <xdr:cNvPr id="22" name="화살표: 왼쪽/오른쪽 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2511,7 +2511,7 @@
         <xdr:cNvPr id="23" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2571,7 +2571,7 @@
         <xdr:cNvPr id="24" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2650,7 +2650,7 @@
         <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2722,7 +2722,7 @@
         <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2794,7 +2794,7 @@
         <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2860,7 +2860,7 @@
         <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2926,7 +2926,7 @@
         <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3054,7 +3054,7 @@
         <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3160,7 +3160,7 @@
         <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3238,7 +3238,7 @@
         <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3316,7 +3316,7 @@
         <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3411,7 +3411,7 @@
         <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3506,7 +3506,7 @@
         <xdr:cNvPr id="12" name="오른쪽 화살표 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3566,7 +3566,7 @@
         <xdr:cNvPr id="13" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3626,7 +3626,7 @@
         <xdr:cNvPr id="14" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3694,7 +3694,7 @@
         <xdr:cNvPr id="15" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3762,7 +3762,7 @@
         <xdr:cNvPr id="16" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3860,7 +3860,7 @@
         <xdr:cNvPr id="17" name="화살표: 왼쪽/오른쪽 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3920,7 +3920,7 @@
         <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4001,7 +4001,7 @@
         <xdr:cNvPr id="20" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4069,7 +4069,7 @@
         <xdr:cNvPr id="21" name="화살표: 왼쪽/오른쪽 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4129,7 +4129,7 @@
         <xdr:cNvPr id="22" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4189,7 +4189,7 @@
         <xdr:cNvPr id="23" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4263,7 +4263,7 @@
         <xdr:cNvPr id="24" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4335,7 +4335,7 @@
         <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4401,7 +4401,7 @@
         <xdr:cNvPr id="26" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4479,7 +4479,7 @@
         <xdr:cNvPr id="27" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4557,7 +4557,7 @@
         <xdr:cNvPr id="28" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4638,7 +4638,7 @@
         <xdr:cNvPr id="29" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4698,7 +4698,7 @@
         <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4764,7 +4764,7 @@
         <xdr:cNvPr id="31" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4836,7 +4836,7 @@
         <xdr:cNvPr id="32" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4904,7 +4904,7 @@
         <xdr:cNvPr id="33" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4964,7 +4964,7 @@
         <xdr:cNvPr id="34" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5024,7 +5024,7 @@
         <xdr:cNvPr id="35" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5084,7 +5084,7 @@
         <xdr:cNvPr id="36" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5184,7 +5184,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5260,7 +5260,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5336,7 +5336,7 @@
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5409,7 +5409,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5488,7 +5488,7 @@
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5551,7 +5551,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5623,7 +5623,7 @@
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5695,7 +5695,7 @@
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5774,7 +5774,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5853,7 +5853,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5932,7 +5932,7 @@
         <xdr:cNvPr id="14" name="사각형: 둥근 모서리 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6A77AD8-C8A0-407A-9C9C-3C7E70C7EA64}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A77AD8-C8A0-407A-9C9C-3C7E70C7EA64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6013,7 +6013,7 @@
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6097,7 +6097,7 @@
         <xdr:cNvPr id="3" name="사각형: 둥근 모서리 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6181,7 +6181,7 @@
         <xdr:cNvPr id="4" name="사각형: 둥근 모서리 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6262,7 +6262,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6361,7 +6361,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6424,7 +6424,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6511,7 +6511,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6583,7 +6583,7 @@
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6662,7 +6662,7 @@
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6741,7 +6741,7 @@
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6820,7 +6820,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6919,7 +6919,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7004,14 +7004,14 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>8964</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>201706</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7019,8 +7019,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1261221" y="639856"/>
-          <a:ext cx="4719918" cy="2286000"/>
+          <a:off x="1260807" y="632402"/>
+          <a:ext cx="4736483" cy="2059446"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7065,7 +7065,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>190x110</a:t>
+            <a:t>190x100</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
             <a:solidFill>
@@ -7095,7 +7095,7 @@
         <xdr:cNvPr id="3" name="사각형: 둥근 모서리 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7171,15 +7171,15 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>201705</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>198782</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="사각형: 둥근 모서리 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7187,8 +7187,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2988050" y="654984"/>
-          <a:ext cx="2984126" cy="2270871"/>
+          <a:off x="2993434" y="647530"/>
+          <a:ext cx="2994893" cy="2036035"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7230,7 +7230,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>120x110</a:t>
+            <a:t>120x100</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
             <a:solidFill>
@@ -7260,7 +7260,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7359,7 +7359,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7422,7 +7422,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7509,7 +7509,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7565,23 +7565,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>138174</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>149476</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80196</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>116347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>39854</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>115858</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>230354</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82728</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7589,7 +7589,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4138674" y="2634259"/>
+          <a:off x="3583739" y="2394064"/>
           <a:ext cx="895593" cy="173447"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -7644,23 +7644,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>202487</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>140025</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>78248</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>98614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>121804</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>122095</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>74544</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7668,8 +7668,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3209074" y="2624808"/>
-          <a:ext cx="664752" cy="189135"/>
+          <a:off x="4575705" y="2376331"/>
+          <a:ext cx="584360" cy="182996"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7724,22 +7724,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>37224</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>164970</xdr:rowOff>
+      <xdr:colOff>12377</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106993</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>231913</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>165651</xdr:rowOff>
+      <xdr:colOff>207066</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107673</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7747,8 +7747,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5266449" y="2679570"/>
-          <a:ext cx="442339" cy="210231"/>
+          <a:off x="5255268" y="2384710"/>
+          <a:ext cx="443168" cy="207746"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7818,7 +7818,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7917,7 +7917,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8314,12 +8314,12 @@
       <c r="F4" s="24">
         <v>2</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="64"/>
     </row>
     <row r="5" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D5" s="6" t="s">
@@ -8458,12 +8458,12 @@
       <c r="L10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="43" t="s">
+      <c r="N10" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="44"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="56"/>
+      <c r="O10" s="59"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="47"/>
     </row>
     <row r="11" spans="4:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="9" t="s">
@@ -8487,14 +8487,14 @@
       <c r="L11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="45" t="s">
+      <c r="N11" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="46"/>
-      <c r="S11" s="57" t="s">
+      <c r="O11" s="57"/>
+      <c r="S11" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="58"/>
+      <c r="T11" s="49"/>
     </row>
     <row r="12" spans="4:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="22" t="s">
@@ -8600,10 +8600,10 @@
       </c>
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="44"/>
+      <c r="J16" s="59"/>
       <c r="N16" s="16">
         <v>5</v>
       </c>
@@ -8614,10 +8614,10 @@
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I17" s="45" t="s">
+      <c r="I17" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="46"/>
+      <c r="J17" s="57"/>
       <c r="N17" s="6">
         <v>6</v>
       </c>
@@ -8673,32 +8673,32 @@
     </row>
     <row r="20" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="44"/>
-      <c r="N21" s="43" t="s">
+      <c r="J21" s="59"/>
+      <c r="N21" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="44"/>
-      <c r="S21" s="55" t="s">
+      <c r="O21" s="59"/>
+      <c r="S21" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="T21" s="56"/>
+      <c r="T21" s="47"/>
     </row>
     <row r="22" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I22" s="49" t="s">
+      <c r="I22" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="50"/>
-      <c r="N22" s="49" t="s">
+      <c r="J22" s="55"/>
+      <c r="N22" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="50"/>
-      <c r="S22" s="57" t="s">
+      <c r="O22" s="55"/>
+      <c r="S22" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="58"/>
+      <c r="T22" s="49"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I23" s="2">
@@ -8742,32 +8742,32 @@
     </row>
     <row r="25" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="N26" s="43" t="s">
+      <c r="J26" s="59"/>
+      <c r="N26" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="O26" s="44"/>
-      <c r="S26" s="61" t="s">
+      <c r="O26" s="59"/>
+      <c r="S26" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="T26" s="62"/>
+      <c r="T26" s="53"/>
     </row>
     <row r="27" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I27" s="45" t="s">
+      <c r="I27" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="46"/>
-      <c r="N27" s="45" t="s">
+      <c r="J27" s="57"/>
+      <c r="N27" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="46"/>
-      <c r="S27" s="59" t="s">
+      <c r="O27" s="57"/>
+      <c r="S27" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="T27" s="60"/>
+      <c r="T27" s="51"/>
     </row>
     <row r="28" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I28" s="2">
@@ -8871,40 +8871,40 @@
     </row>
     <row r="33" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I34" s="43" t="s">
+      <c r="I34" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="J34" s="44"/>
-      <c r="N34" s="43" t="s">
+      <c r="J34" s="59"/>
+      <c r="N34" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="O34" s="44"/>
-      <c r="S34" s="61" t="s">
+      <c r="O34" s="59"/>
+      <c r="S34" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="62"/>
-      <c r="V34" s="53" t="s">
+      <c r="T34" s="53"/>
+      <c r="V34" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="W34" s="54"/>
+      <c r="W34" s="45"/>
     </row>
     <row r="35" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I35" s="45" t="s">
+      <c r="I35" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="46"/>
-      <c r="N35" s="47" t="s">
+      <c r="J35" s="57"/>
+      <c r="N35" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="O35" s="48"/>
-      <c r="S35" s="49" t="s">
+      <c r="O35" s="61"/>
+      <c r="S35" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="T35" s="50"/>
-      <c r="V35" s="51" t="s">
+      <c r="T35" s="55"/>
+      <c r="V35" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="W35" s="52"/>
+      <c r="W35" s="43"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I36" s="2">
@@ -9005,10 +9005,10 @@
       </c>
     </row>
     <row r="40" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I40" s="43" t="s">
+      <c r="I40" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="44"/>
+      <c r="J40" s="59"/>
       <c r="N40" s="9">
         <v>5</v>
       </c>
@@ -9029,10 +9029,10 @@
       </c>
     </row>
     <row r="41" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I41" s="45" t="s">
+      <c r="I41" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="46"/>
+      <c r="J41" s="57"/>
     </row>
     <row r="42" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I42" s="2">
@@ -9041,10 +9041,10 @@
       <c r="J42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N42" s="43" t="s">
+      <c r="N42" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O42" s="44"/>
+      <c r="O42" s="59"/>
     </row>
     <row r="43" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I43" s="9">
@@ -9053,10 +9053,10 @@
       <c r="J43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N43" s="45" t="s">
+      <c r="N43" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="O43" s="46"/>
+      <c r="O43" s="57"/>
     </row>
     <row r="44" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N44" s="2">
@@ -9067,10 +9067,10 @@
       </c>
     </row>
     <row r="45" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I45" s="43" t="s">
+      <c r="I45" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="44"/>
+      <c r="J45" s="59"/>
       <c r="N45" s="9">
         <v>2</v>
       </c>
@@ -9079,10 +9079,10 @@
       </c>
     </row>
     <row r="46" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I46" s="45" t="s">
+      <c r="I46" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="46"/>
+      <c r="J46" s="57"/>
     </row>
     <row r="47" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I47" s="2">
@@ -9091,10 +9091,10 @@
       <c r="J47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N47" s="43" t="s">
+      <c r="N47" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="O47" s="44"/>
+      <c r="O47" s="59"/>
     </row>
     <row r="48" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I48" s="9">
@@ -9103,10 +9103,10 @@
       <c r="J48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N48" s="45" t="s">
+      <c r="N48" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="O48" s="46"/>
+      <c r="O48" s="57"/>
     </row>
     <row r="49" spans="11:15" x14ac:dyDescent="0.3">
       <c r="N49" s="2">
@@ -9134,22 +9134,13 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="I41:J41"/>
     <mergeCell ref="N34:O34"/>
@@ -9162,13 +9153,22 @@
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S35:T35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9181,7 +9181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
@@ -9263,38 +9263,38 @@
       <c r="D7" s="26">
         <v>5</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="J7" s="43" t="s">
+      <c r="H7" s="59"/>
+      <c r="J7" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="44"/>
-      <c r="P7" s="43" t="s">
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="59"/>
+      <c r="P7" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="44"/>
-      <c r="U7" s="43" t="s">
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="59"/>
+      <c r="U7" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="V7" s="44"/>
-      <c r="Y7" s="53" t="s">
+      <c r="V7" s="59"/>
+      <c r="Y7" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="54"/>
-      <c r="AB7" s="61" t="s">
+      <c r="Z7" s="45"/>
+      <c r="AB7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="AC7" s="62"/>
-      <c r="AF7" s="61" t="s">
+      <c r="AC7" s="53"/>
+      <c r="AF7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="AG7" s="62"/>
+      <c r="AG7" s="53"/>
     </row>
     <row r="8" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
@@ -9306,38 +9306,38 @@
       <c r="D8" s="26">
         <v>35</v>
       </c>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="J8" s="63" t="s">
+      <c r="H8" s="55"/>
+      <c r="J8" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="64"/>
-      <c r="P8" s="63" t="s">
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="66"/>
+      <c r="P8" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="64"/>
-      <c r="U8" s="45" t="s">
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="66"/>
+      <c r="U8" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="V8" s="46"/>
-      <c r="Y8" s="51" t="s">
+      <c r="V8" s="57"/>
+      <c r="Y8" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="52"/>
-      <c r="AB8" s="49" t="s">
+      <c r="Z8" s="43"/>
+      <c r="AB8" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="AC8" s="50"/>
-      <c r="AF8" s="49" t="s">
+      <c r="AC8" s="55"/>
+      <c r="AF8" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="AG8" s="50"/>
+      <c r="AG8" s="55"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -9532,14 +9532,14 @@
         <f>SUM(D4:D11)</f>
         <v>150.19999999999999</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="59"/>
       <c r="J12" s="6">
         <v>7</v>
       </c>
-      <c r="K12" s="67" t="s">
+      <c r="K12" s="40" t="s">
         <v>27</v>
       </c>
       <c r="L12" s="1">
@@ -9551,7 +9551,7 @@
       <c r="P12" s="6">
         <v>7</v>
       </c>
-      <c r="Q12" s="67" t="s">
+      <c r="Q12" s="40" t="s">
         <v>27</v>
       </c>
       <c r="R12" s="1">
@@ -9586,10 +9586,10 @@
       </c>
     </row>
     <row r="13" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="46"/>
+      <c r="H13" s="57"/>
       <c r="J13" s="6">
         <v>9</v>
       </c>
@@ -9702,14 +9702,14 @@
       <c r="S15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U15" s="43" t="s">
+      <c r="U15" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="V15" s="44"/>
-      <c r="Y15" s="43" t="s">
+      <c r="V15" s="59"/>
+      <c r="Y15" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="Z15" s="44"/>
+      <c r="Z15" s="59"/>
     </row>
     <row r="16" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="6">
@@ -9734,14 +9734,14 @@
         <v>16</v>
       </c>
       <c r="S16" s="8"/>
-      <c r="U16" s="45" t="s">
+      <c r="U16" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="V16" s="46"/>
-      <c r="Y16" s="45" t="s">
+      <c r="V16" s="57"/>
+      <c r="Y16" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="Z16" s="46"/>
+      <c r="Z16" s="57"/>
     </row>
     <row r="17" spans="7:26" x14ac:dyDescent="0.3">
       <c r="G17" s="6">
@@ -9833,40 +9833,40 @@
     </row>
     <row r="19" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="7:26" x14ac:dyDescent="0.3">
-      <c r="G20" s="43" t="s">
+      <c r="G20" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="L20" s="43" t="s">
+      <c r="H20" s="59"/>
+      <c r="L20" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="44"/>
-      <c r="U20" s="43" t="s">
+      <c r="M20" s="59"/>
+      <c r="U20" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="V20" s="44"/>
-      <c r="Y20" s="43" t="s">
+      <c r="V20" s="59"/>
+      <c r="Y20" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="Z20" s="44"/>
+      <c r="Z20" s="59"/>
     </row>
     <row r="21" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="46"/>
-      <c r="L21" s="45" t="s">
+      <c r="H21" s="57"/>
+      <c r="L21" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="U21" s="45" t="s">
+      <c r="M21" s="57"/>
+      <c r="U21" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="V21" s="46"/>
-      <c r="Y21" s="45" t="s">
+      <c r="V21" s="57"/>
+      <c r="Y21" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="46"/>
+      <c r="Z21" s="57"/>
     </row>
     <row r="22" spans="7:26" x14ac:dyDescent="0.3">
       <c r="G22" s="2">
@@ -9941,10 +9941,10 @@
       </c>
     </row>
     <row r="25" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L25" s="43" t="s">
+      <c r="L25" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="44"/>
+      <c r="M25" s="59"/>
       <c r="U25" s="6">
         <v>4</v>
       </c>
@@ -9959,14 +9959,14 @@
       </c>
     </row>
     <row r="26" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G26" s="43" t="s">
+      <c r="G26" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="44"/>
-      <c r="L26" s="45" t="s">
+      <c r="H26" s="59"/>
+      <c r="L26" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="46"/>
+      <c r="M26" s="57"/>
       <c r="U26" s="9">
         <v>5</v>
       </c>
@@ -9981,10 +9981,10 @@
       </c>
     </row>
     <row r="27" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="45" t="s">
+      <c r="G27" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="46"/>
+      <c r="H27" s="57"/>
       <c r="L27" s="2">
         <v>1</v>
       </c>
@@ -10015,26 +10015,26 @@
       </c>
     </row>
     <row r="30" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L30" s="43" t="s">
+      <c r="L30" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="M30" s="44"/>
+      <c r="M30" s="59"/>
     </row>
     <row r="31" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="43" t="s">
+      <c r="G31" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="44"/>
-      <c r="L31" s="63" t="s">
+      <c r="H31" s="59"/>
+      <c r="L31" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M31" s="64"/>
+      <c r="M31" s="66"/>
     </row>
     <row r="32" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="46"/>
+      <c r="H32" s="57"/>
       <c r="L32" s="2">
         <v>1</v>
       </c>
@@ -10065,34 +10065,34 @@
       </c>
     </row>
     <row r="35" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L35" s="43" t="s">
+      <c r="L35" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="44"/>
-      <c r="AF35" s="43" t="s">
+      <c r="M35" s="59"/>
+      <c r="AF35" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AG35" s="44"/>
+      <c r="AG35" s="59"/>
     </row>
     <row r="36" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G36" s="43" t="s">
+      <c r="G36" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="H36" s="44"/>
-      <c r="L36" s="63" t="s">
+      <c r="H36" s="59"/>
+      <c r="L36" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M36" s="64"/>
-      <c r="AF36" s="63" t="s">
+      <c r="M36" s="66"/>
+      <c r="AF36" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AG36" s="64"/>
+      <c r="AG36" s="66"/>
     </row>
     <row r="37" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G37" s="45" t="s">
+      <c r="G37" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="46"/>
+      <c r="H37" s="57"/>
       <c r="L37" s="2">
         <v>1</v>
       </c>
@@ -10135,24 +10135,24 @@
       </c>
     </row>
     <row r="40" spans="7:33" x14ac:dyDescent="0.3">
-      <c r="L40" s="43" t="s">
+      <c r="L40" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="M40" s="44"/>
-      <c r="AF40" s="43" t="s">
+      <c r="M40" s="59"/>
+      <c r="AF40" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AG40" s="44"/>
+      <c r="AG40" s="59"/>
     </row>
     <row r="41" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L41" s="63" t="s">
+      <c r="L41" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M41" s="64"/>
-      <c r="AF41" s="63" t="s">
+      <c r="M41" s="66"/>
+      <c r="AF41" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AG41" s="64"/>
+      <c r="AG41" s="66"/>
     </row>
     <row r="42" spans="7:33" x14ac:dyDescent="0.3">
       <c r="L42" s="2">
@@ -10184,12 +10184,12 @@
     </row>
     <row r="45" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J46" s="40" t="s">
+      <c r="J46" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="42"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="64"/>
     </row>
     <row r="47" spans="7:33" x14ac:dyDescent="0.3">
       <c r="J47" s="2">
@@ -10204,10 +10204,10 @@
       <c r="M47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y47" s="43" t="s">
+      <c r="Y47" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="Z47" s="44"/>
+      <c r="Z47" s="59"/>
     </row>
     <row r="48" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J48" s="6">
@@ -10222,10 +10222,10 @@
       <c r="M48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y48" s="63" t="s">
+      <c r="Y48" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="Z48" s="64"/>
+      <c r="Z48" s="66"/>
     </row>
     <row r="49" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J49" s="6">
@@ -10353,12 +10353,38 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="AF35:AG35"/>
-    <mergeCell ref="AF36:AG36"/>
-    <mergeCell ref="AF40:AG40"/>
-    <mergeCell ref="AF41:AG41"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y47:Z47"/>
+    <mergeCell ref="Y48:Z48"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G36:H36"/>
@@ -10370,38 +10396,12 @@
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="L31:M31"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="Y47:Z47"/>
-    <mergeCell ref="Y48:Z48"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="AF35:AG35"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AF40:AG40"/>
+    <mergeCell ref="AF41:AG41"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AF8:AG8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11168,8 +11168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11512,7 +11512,7 @@
       <c r="D9" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="41">
         <f>(E7*E8)^0.5</f>
         <v>122.47448713915891</v>
       </c>
@@ -11524,7 +11524,7 @@
       <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="41">
         <f>(E9/0.707)*2</f>
         <v>346.46248129889369</v>
       </c>

</xml_diff>

<commit_message>
[10/28] PCB artwork - Home
</commit_message>
<xml_diff>
--- a/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
+++ b/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RFGEN V2.0" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,12 +477,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -844,8 +838,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,49 +908,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -964,7 +957,7 @@
         <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,7 +1029,7 @@
         <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1108,7 +1101,7 @@
         <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1174,7 +1167,7 @@
         <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1240,7 +1233,7 @@
         <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,7 +1361,7 @@
         <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1467,7 @@
         <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1552,7 +1545,7 @@
         <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1630,7 +1623,7 @@
         <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1725,7 +1718,7 @@
         <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1820,7 +1813,7 @@
         <xdr:cNvPr id="8" name="오른쪽 화살표 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,7 +1873,7 @@
         <xdr:cNvPr id="14" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1940,7 +1933,7 @@
         <xdr:cNvPr id="15" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2008,7 +2001,7 @@
         <xdr:cNvPr id="16" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2076,7 +2069,7 @@
         <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2167,7 @@
         <xdr:cNvPr id="13" name="화살표: 왼쪽/오른쪽 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2234,7 +2227,7 @@
         <xdr:cNvPr id="19" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2315,7 +2308,7 @@
         <xdr:cNvPr id="20" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2383,7 +2376,7 @@
         <xdr:cNvPr id="21" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2451,7 +2444,7 @@
         <xdr:cNvPr id="22" name="화살표: 왼쪽/오른쪽 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2511,7 +2504,7 @@
         <xdr:cNvPr id="23" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2571,7 +2564,7 @@
         <xdr:cNvPr id="24" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2650,7 +2643,7 @@
         <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2722,7 +2715,7 @@
         <xdr:cNvPr id="3" name="모서리가 둥근 직사각형 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2794,7 +2787,7 @@
         <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2860,7 +2853,7 @@
         <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2926,7 +2919,7 @@
         <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3054,7 +3047,7 @@
         <xdr:cNvPr id="7" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3160,7 +3153,7 @@
         <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3238,7 +3231,7 @@
         <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3316,7 +3309,7 @@
         <xdr:cNvPr id="10" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3411,7 +3404,7 @@
         <xdr:cNvPr id="11" name="모서리가 둥근 직사각형 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3506,7 +3499,7 @@
         <xdr:cNvPr id="12" name="오른쪽 화살표 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3566,7 +3559,7 @@
         <xdr:cNvPr id="13" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3626,7 +3619,7 @@
         <xdr:cNvPr id="14" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3694,7 +3687,7 @@
         <xdr:cNvPr id="15" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3762,7 +3755,7 @@
         <xdr:cNvPr id="16" name="모서리가 둥근 직사각형 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3860,7 +3853,7 @@
         <xdr:cNvPr id="17" name="화살표: 왼쪽/오른쪽 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3920,7 +3913,7 @@
         <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4001,7 +3994,7 @@
         <xdr:cNvPr id="20" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4069,7 +4062,7 @@
         <xdr:cNvPr id="21" name="화살표: 왼쪽/오른쪽 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4129,7 +4122,7 @@
         <xdr:cNvPr id="22" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4189,7 +4182,7 @@
         <xdr:cNvPr id="23" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4263,7 +4256,7 @@
         <xdr:cNvPr id="24" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4335,7 +4328,7 @@
         <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4401,7 +4394,7 @@
         <xdr:cNvPr id="26" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4479,7 +4472,7 @@
         <xdr:cNvPr id="27" name="모서리가 둥근 직사각형 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4557,7 +4550,7 @@
         <xdr:cNvPr id="28" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4638,7 +4631,7 @@
         <xdr:cNvPr id="29" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4698,7 +4691,7 @@
         <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4764,7 +4757,7 @@
         <xdr:cNvPr id="31" name="모서리가 둥근 직사각형 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4836,7 +4829,7 @@
         <xdr:cNvPr id="32" name="오른쪽 화살표 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4904,7 +4897,7 @@
         <xdr:cNvPr id="33" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4964,7 +4957,7 @@
         <xdr:cNvPr id="34" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5024,7 +5017,7 @@
         <xdr:cNvPr id="35" name="오른쪽 화살표 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5084,7 +5077,7 @@
         <xdr:cNvPr id="36" name="모서리가 둥근 직사각형 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5184,7 +5177,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5260,7 +5253,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5336,7 +5329,7 @@
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5409,7 +5402,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5488,7 +5481,7 @@
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5551,7 +5544,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5623,7 +5616,7 @@
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5695,7 +5688,7 @@
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5774,7 +5767,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5853,7 +5846,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5932,7 +5925,7 @@
         <xdr:cNvPr id="14" name="사각형: 둥근 모서리 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A77AD8-C8A0-407A-9C9C-3C7E70C7EA64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6A77AD8-C8A0-407A-9C9C-3C7E70C7EA64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6013,7 +6006,7 @@
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6097,7 +6090,7 @@
         <xdr:cNvPr id="3" name="사각형: 둥근 모서리 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6181,7 +6174,7 @@
         <xdr:cNvPr id="4" name="사각형: 둥근 모서리 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6262,7 +6255,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6361,7 +6354,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6424,7 +6417,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6511,7 +6504,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6583,7 +6576,7 @@
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6662,7 +6655,7 @@
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6741,7 +6734,7 @@
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6820,7 +6813,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6919,7 +6912,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7011,7 +7004,7 @@
         <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{435C5B1E-CB63-4117-8D00-50BC1A27F7F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7095,7 +7088,7 @@
         <xdr:cNvPr id="3" name="사각형: 둥근 모서리 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BF26FDA-60DD-42E9-BEEA-EFF023C1EF3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7179,7 +7172,7 @@
         <xdr:cNvPr id="4" name="사각형: 둥근 모서리 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A05A2CB9-E356-4835-9C98-02FC047B45C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7260,7 +7253,7 @@
         <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACE4500D-F764-43EA-820B-86881BB81791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7359,7 +7352,7 @@
         <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FFB1F820-C80B-45BF-8D1C-725C4F73AA81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7422,7 +7415,7 @@
         <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0BBFD670-C20F-432B-9F99-791457FDC723}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7509,7 +7502,7 @@
         <xdr:cNvPr id="8" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F12DE4EF-2976-48E0-BC1C-AF49AD3605D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7581,7 +7574,7 @@
         <xdr:cNvPr id="9" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE372FF0-C4E4-4086-8560-F983F0762A74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7660,7 +7653,7 @@
         <xdr:cNvPr id="10" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50E22FFC-9E34-486B-9169-705394D54359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7739,7 +7732,7 @@
         <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B79A87BC-2F88-42BD-9493-3EFB5DE32D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7818,7 +7811,7 @@
         <xdr:cNvPr id="12" name="사각형: 둥근 모서리 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD62FA63-E115-4216-A3BD-755CDA78680C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7917,7 +7910,7 @@
         <xdr:cNvPr id="13" name="사각형: 둥근 모서리 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F131502-0C5F-4969-9F15-D733E96A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8314,12 +8307,12 @@
       <c r="F4" s="24">
         <v>2</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="64"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D5" s="6" t="s">
@@ -8458,12 +8451,12 @@
       <c r="L10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="58" t="s">
+      <c r="N10" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="59"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="47"/>
+      <c r="O10" s="45"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="57"/>
     </row>
     <row r="11" spans="4:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="9" t="s">
@@ -8487,14 +8480,14 @@
       <c r="L11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="56" t="s">
+      <c r="N11" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="57"/>
-      <c r="S11" s="48" t="s">
+      <c r="O11" s="47"/>
+      <c r="S11" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="49"/>
+      <c r="T11" s="59"/>
     </row>
     <row r="12" spans="4:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="22" t="s">
@@ -8600,10 +8593,10 @@
       </c>
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="I16" s="58" t="s">
+      <c r="I16" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="45"/>
       <c r="N16" s="16">
         <v>5</v>
       </c>
@@ -8614,10 +8607,10 @@
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="57"/>
+      <c r="J17" s="47"/>
       <c r="N17" s="6">
         <v>6</v>
       </c>
@@ -8673,32 +8666,32 @@
     </row>
     <row r="20" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I21" s="58" t="s">
+      <c r="I21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="59"/>
-      <c r="N21" s="58" t="s">
+      <c r="J21" s="45"/>
+      <c r="N21" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="59"/>
-      <c r="S21" s="46" t="s">
+      <c r="O21" s="45"/>
+      <c r="S21" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="T21" s="47"/>
+      <c r="T21" s="57"/>
     </row>
     <row r="22" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I22" s="54" t="s">
+      <c r="I22" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="55"/>
-      <c r="N22" s="54" t="s">
+      <c r="J22" s="51"/>
+      <c r="N22" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="55"/>
-      <c r="S22" s="48" t="s">
+      <c r="O22" s="51"/>
+      <c r="S22" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="49"/>
+      <c r="T22" s="59"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I23" s="2">
@@ -8742,32 +8735,32 @@
     </row>
     <row r="25" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I26" s="58" t="s">
+      <c r="I26" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="59"/>
-      <c r="N26" s="58" t="s">
+      <c r="J26" s="45"/>
+      <c r="N26" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O26" s="59"/>
-      <c r="S26" s="52" t="s">
+      <c r="O26" s="45"/>
+      <c r="S26" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="T26" s="53"/>
+      <c r="T26" s="63"/>
     </row>
     <row r="27" spans="9:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I27" s="56" t="s">
+      <c r="I27" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="57"/>
-      <c r="N27" s="56" t="s">
+      <c r="J27" s="47"/>
+      <c r="N27" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="57"/>
-      <c r="S27" s="50" t="s">
+      <c r="O27" s="47"/>
+      <c r="S27" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="T27" s="51"/>
+      <c r="T27" s="61"/>
     </row>
     <row r="28" spans="9:20" x14ac:dyDescent="0.3">
       <c r="I28" s="2">
@@ -8871,40 +8864,40 @@
     </row>
     <row r="33" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="9:23" x14ac:dyDescent="0.3">
-      <c r="I34" s="58" t="s">
+      <c r="I34" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="J34" s="59"/>
-      <c r="N34" s="58" t="s">
+      <c r="J34" s="45"/>
+      <c r="N34" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="O34" s="59"/>
-      <c r="S34" s="52" t="s">
+      <c r="O34" s="45"/>
+      <c r="S34" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="53"/>
-      <c r="V34" s="44" t="s">
+      <c r="T34" s="63"/>
+      <c r="V34" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="W34" s="45"/>
+      <c r="W34" s="55"/>
     </row>
     <row r="35" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="57"/>
-      <c r="N35" s="60" t="s">
+      <c r="J35" s="47"/>
+      <c r="N35" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="O35" s="61"/>
-      <c r="S35" s="54" t="s">
+      <c r="O35" s="49"/>
+      <c r="S35" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="T35" s="55"/>
-      <c r="V35" s="42" t="s">
+      <c r="T35" s="51"/>
+      <c r="V35" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="W35" s="43"/>
+      <c r="W35" s="53"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I36" s="2">
@@ -9005,10 +8998,10 @@
       </c>
     </row>
     <row r="40" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I40" s="58" t="s">
+      <c r="I40" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="59"/>
+      <c r="J40" s="45"/>
       <c r="N40" s="9">
         <v>5</v>
       </c>
@@ -9029,10 +9022,10 @@
       </c>
     </row>
     <row r="41" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I41" s="56" t="s">
+      <c r="I41" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="57"/>
+      <c r="J41" s="47"/>
     </row>
     <row r="42" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I42" s="2">
@@ -9041,10 +9034,10 @@
       <c r="J42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N42" s="58" t="s">
+      <c r="N42" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="O42" s="59"/>
+      <c r="O42" s="45"/>
     </row>
     <row r="43" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I43" s="9">
@@ -9053,10 +9046,10 @@
       <c r="J43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N43" s="56" t="s">
+      <c r="N43" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="O43" s="57"/>
+      <c r="O43" s="47"/>
     </row>
     <row r="44" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N44" s="2">
@@ -9067,10 +9060,10 @@
       </c>
     </row>
     <row r="45" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I45" s="58" t="s">
+      <c r="I45" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="59"/>
+      <c r="J45" s="45"/>
       <c r="N45" s="9">
         <v>2</v>
       </c>
@@ -9079,10 +9072,10 @@
       </c>
     </row>
     <row r="46" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I46" s="56" t="s">
+      <c r="I46" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="57"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I47" s="2">
@@ -9091,10 +9084,10 @@
       <c r="J47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N47" s="58" t="s">
+      <c r="N47" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="O47" s="59"/>
+      <c r="O47" s="45"/>
     </row>
     <row r="48" spans="9:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I48" s="9">
@@ -9103,10 +9096,10 @@
       <c r="J48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N48" s="56" t="s">
+      <c r="N48" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="O48" s="57"/>
+      <c r="O48" s="47"/>
     </row>
     <row r="49" spans="11:15" x14ac:dyDescent="0.3">
       <c r="N49" s="2">
@@ -9134,13 +9127,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="V34:W34"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="I41:J41"/>
     <mergeCell ref="N34:O34"/>
@@ -9153,22 +9155,13 @@
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I22:J22"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="V35:W35"/>
-    <mergeCell ref="V34:W34"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9181,8 +9174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG56"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9263,38 +9256,38 @@
       <c r="D7" s="26">
         <v>5</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="59"/>
-      <c r="J7" s="58" t="s">
+      <c r="H7" s="45"/>
+      <c r="J7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="59"/>
-      <c r="P7" s="58" t="s">
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="45"/>
+      <c r="P7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="59"/>
-      <c r="U7" s="58" t="s">
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="45"/>
+      <c r="U7" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="V7" s="59"/>
-      <c r="Y7" s="44" t="s">
+      <c r="V7" s="45"/>
+      <c r="Y7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="45"/>
-      <c r="AB7" s="52" t="s">
+      <c r="Z7" s="55"/>
+      <c r="AB7" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="AC7" s="53"/>
-      <c r="AF7" s="52" t="s">
+      <c r="AC7" s="63"/>
+      <c r="AF7" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="AG7" s="53"/>
+      <c r="AG7" s="63"/>
     </row>
     <row r="8" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
@@ -9306,38 +9299,38 @@
       <c r="D8" s="26">
         <v>35</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="55"/>
-      <c r="J8" s="65" t="s">
+      <c r="H8" s="51"/>
+      <c r="J8" s="64" t="s">
         <v>62</v>
       </c>
       <c r="K8" s="67"/>
       <c r="L8" s="67"/>
-      <c r="M8" s="66"/>
-      <c r="P8" s="65" t="s">
+      <c r="M8" s="65"/>
+      <c r="P8" s="64" t="s">
         <v>62</v>
       </c>
       <c r="Q8" s="67"/>
       <c r="R8" s="67"/>
-      <c r="S8" s="66"/>
-      <c r="U8" s="56" t="s">
+      <c r="S8" s="65"/>
+      <c r="U8" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="V8" s="57"/>
-      <c r="Y8" s="42" t="s">
+      <c r="V8" s="47"/>
+      <c r="Y8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="43"/>
-      <c r="AB8" s="54" t="s">
+      <c r="Z8" s="53"/>
+      <c r="AB8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AC8" s="55"/>
-      <c r="AF8" s="54" t="s">
+      <c r="AC8" s="51"/>
+      <c r="AF8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AG8" s="55"/>
+      <c r="AG8" s="51"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -9532,14 +9525,14 @@
         <f>SUM(D4:D11)</f>
         <v>150.19999999999999</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="59"/>
+      <c r="H12" s="45"/>
       <c r="J12" s="6">
         <v>7</v>
       </c>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="13" t="s">
         <v>27</v>
       </c>
       <c r="L12" s="1">
@@ -9551,7 +9544,7 @@
       <c r="P12" s="6">
         <v>7</v>
       </c>
-      <c r="Q12" s="40" t="s">
+      <c r="Q12" s="13" t="s">
         <v>27</v>
       </c>
       <c r="R12" s="1">
@@ -9586,10 +9579,10 @@
       </c>
     </row>
     <row r="13" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="57"/>
+      <c r="H13" s="47"/>
       <c r="J13" s="6">
         <v>9</v>
       </c>
@@ -9702,14 +9695,14 @@
       <c r="S15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U15" s="58" t="s">
+      <c r="U15" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="V15" s="59"/>
-      <c r="Y15" s="58" t="s">
+      <c r="V15" s="45"/>
+      <c r="Y15" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="Z15" s="59"/>
+      <c r="Z15" s="45"/>
     </row>
     <row r="16" spans="2:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="6">
@@ -9734,14 +9727,14 @@
         <v>16</v>
       </c>
       <c r="S16" s="8"/>
-      <c r="U16" s="56" t="s">
+      <c r="U16" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="V16" s="57"/>
-      <c r="Y16" s="56" t="s">
+      <c r="V16" s="47"/>
+      <c r="Y16" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="Z16" s="57"/>
+      <c r="Z16" s="47"/>
     </row>
     <row r="17" spans="7:26" x14ac:dyDescent="0.3">
       <c r="G17" s="6">
@@ -9833,40 +9826,40 @@
     </row>
     <row r="19" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="7:26" x14ac:dyDescent="0.3">
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="59"/>
-      <c r="L20" s="58" t="s">
+      <c r="H20" s="45"/>
+      <c r="L20" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="59"/>
-      <c r="U20" s="58" t="s">
+      <c r="M20" s="45"/>
+      <c r="U20" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="V20" s="59"/>
-      <c r="Y20" s="58" t="s">
+      <c r="V20" s="45"/>
+      <c r="Y20" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="Z20" s="59"/>
+      <c r="Z20" s="45"/>
     </row>
     <row r="21" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G21" s="56" t="s">
+      <c r="G21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="L21" s="56" t="s">
+      <c r="H21" s="47"/>
+      <c r="L21" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="57"/>
-      <c r="U21" s="56" t="s">
+      <c r="M21" s="47"/>
+      <c r="U21" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="V21" s="57"/>
-      <c r="Y21" s="56" t="s">
+      <c r="V21" s="47"/>
+      <c r="Y21" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="57"/>
+      <c r="Z21" s="47"/>
     </row>
     <row r="22" spans="7:26" x14ac:dyDescent="0.3">
       <c r="G22" s="2">
@@ -9941,10 +9934,10 @@
       </c>
     </row>
     <row r="25" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L25" s="58" t="s">
+      <c r="L25" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="59"/>
+      <c r="M25" s="45"/>
       <c r="U25" s="6">
         <v>4</v>
       </c>
@@ -9959,14 +9952,14 @@
       </c>
     </row>
     <row r="26" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="59"/>
-      <c r="L26" s="56" t="s">
+      <c r="H26" s="45"/>
+      <c r="L26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="57"/>
+      <c r="M26" s="47"/>
       <c r="U26" s="9">
         <v>5</v>
       </c>
@@ -9981,10 +9974,10 @@
       </c>
     </row>
     <row r="27" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="57"/>
+      <c r="H27" s="47"/>
       <c r="L27" s="2">
         <v>1</v>
       </c>
@@ -10015,26 +10008,26 @@
       </c>
     </row>
     <row r="30" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L30" s="58" t="s">
+      <c r="L30" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="M30" s="59"/>
+      <c r="M30" s="45"/>
     </row>
     <row r="31" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="58" t="s">
+      <c r="G31" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="59"/>
-      <c r="L31" s="65" t="s">
+      <c r="H31" s="45"/>
+      <c r="L31" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="M31" s="66"/>
+      <c r="M31" s="65"/>
     </row>
     <row r="32" spans="7:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="57"/>
+      <c r="H32" s="47"/>
       <c r="L32" s="2">
         <v>1</v>
       </c>
@@ -10065,34 +10058,34 @@
       </c>
     </row>
     <row r="35" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L35" s="58" t="s">
+      <c r="L35" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="M35" s="59"/>
-      <c r="AF35" s="58" t="s">
+      <c r="M35" s="45"/>
+      <c r="AF35" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="AG35" s="59"/>
+      <c r="AG35" s="45"/>
     </row>
     <row r="36" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G36" s="58" t="s">
+      <c r="G36" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H36" s="59"/>
-      <c r="L36" s="65" t="s">
+      <c r="H36" s="45"/>
+      <c r="L36" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="M36" s="66"/>
-      <c r="AF36" s="65" t="s">
+      <c r="M36" s="65"/>
+      <c r="AF36" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AG36" s="66"/>
+      <c r="AG36" s="65"/>
     </row>
     <row r="37" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G37" s="56" t="s">
+      <c r="G37" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="57"/>
+      <c r="H37" s="47"/>
       <c r="L37" s="2">
         <v>1</v>
       </c>
@@ -10135,24 +10128,24 @@
       </c>
     </row>
     <row r="40" spans="7:33" x14ac:dyDescent="0.3">
-      <c r="L40" s="58" t="s">
+      <c r="L40" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="M40" s="59"/>
-      <c r="AF40" s="58" t="s">
+      <c r="M40" s="45"/>
+      <c r="AF40" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="AG40" s="59"/>
+      <c r="AG40" s="45"/>
     </row>
     <row r="41" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L41" s="65" t="s">
+      <c r="L41" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="M41" s="66"/>
-      <c r="AF41" s="65" t="s">
+      <c r="M41" s="65"/>
+      <c r="AF41" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AG41" s="66"/>
+      <c r="AG41" s="65"/>
     </row>
     <row r="42" spans="7:33" x14ac:dyDescent="0.3">
       <c r="L42" s="2">
@@ -10184,12 +10177,12 @@
     </row>
     <row r="45" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J46" s="62" t="s">
+      <c r="J46" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="K46" s="63"/>
-      <c r="L46" s="63"/>
-      <c r="M46" s="64"/>
+      <c r="K46" s="42"/>
+      <c r="L46" s="42"/>
+      <c r="M46" s="43"/>
     </row>
     <row r="47" spans="7:33" x14ac:dyDescent="0.3">
       <c r="J47" s="2">
@@ -10204,10 +10197,10 @@
       <c r="M47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y47" s="58" t="s">
+      <c r="Y47" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="Z47" s="59"/>
+      <c r="Z47" s="45"/>
     </row>
     <row r="48" spans="7:33" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J48" s="6">
@@ -10222,10 +10215,10 @@
       <c r="M48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y48" s="65" t="s">
+      <c r="Y48" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="Z48" s="66"/>
+      <c r="Z48" s="65"/>
     </row>
     <row r="49" spans="10:26" x14ac:dyDescent="0.3">
       <c r="J49" s="6">
@@ -10353,6 +10346,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="AF35:AG35"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AF40:AG40"/>
+    <mergeCell ref="AF41:AG41"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="Y47:Z47"/>
+    <mergeCell ref="Y48:Z48"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="J7:M7"/>
     <mergeCell ref="J46:M46"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="U20:V20"/>
@@ -10364,44 +10390,11 @@
     <mergeCell ref="L41:M41"/>
     <mergeCell ref="U21:V21"/>
     <mergeCell ref="L26:M26"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="Y47:Z47"/>
-    <mergeCell ref="Y48:Z48"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="J7:M7"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="AF35:AG35"/>
-    <mergeCell ref="AF36:AG36"/>
-    <mergeCell ref="AF40:AG40"/>
-    <mergeCell ref="AF41:AG41"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="AF8:AG8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11168,8 +11161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11512,7 +11505,7 @@
       <c r="D9" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="40">
         <f>(E7*E8)^0.5</f>
         <v>122.47448713915891</v>
       </c>
@@ -11524,7 +11517,7 @@
       <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="40">
         <f>(E9/0.707)*2</f>
         <v>346.46248129889369</v>
       </c>

</xml_diff>

<commit_message>
[11/6]RF PCB update - company work
</commit_message>
<xml_diff>
--- a/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
+++ b/0_Block Diagram/Plasma_Gen_Block Diagram_V2.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A86437-B45E-42DB-85FD-4EF34BF6FEFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391AC156-EF85-4C3F-BC87-C8770050644B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RFGEN V2.0" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Block1" sheetId="2" r:id="rId3"/>
     <sheet name="Block2" sheetId="5" r:id="rId4"/>
     <sheet name="Block3" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Block1106" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="113">
   <si>
     <t>+12V</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,6 +408,70 @@
   </si>
   <si>
     <t>TH-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heat Sink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bracket T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF HS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR HS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF FAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWR FAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50x50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80x80</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -821,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -866,6 +931,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -959,12 +1031,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -7420,16 +7486,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>58</xdr:col>
-      <xdr:colOff>242043</xdr:colOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>89643</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>57881</xdr:rowOff>
+      <xdr:rowOff>219246</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>647285</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>74543</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>494885</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>11791</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7444,8 +7510,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17244168" y="3829781"/>
-          <a:ext cx="2462642" cy="4207662"/>
+          <a:off x="16297831" y="4253364"/>
+          <a:ext cx="2422301" cy="4499015"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7582,16 +7648,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>614610</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>126286</xdr:rowOff>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>211198</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>72497</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>278295</xdr:colOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>547236</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>41412</xdr:rowOff>
+      <xdr:rowOff>211741</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7606,8 +7672,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16930935" y="4736386"/>
-          <a:ext cx="2406885" cy="3267926"/>
+          <a:off x="16419386" y="5227203"/>
+          <a:ext cx="2353097" cy="3501009"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -9117,6 +9183,2930 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>233082</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>26895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>216905</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>212036</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="사각형: 둥근 모서리 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEE3FFA3-CD32-4B6E-AD2D-9106FD917DB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1237129" y="3164542"/>
+          <a:ext cx="2404294" cy="5339847"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3334"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>RF</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>240x100</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>242046</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>8964</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8FD2A3-BA11-44B5-941B-9E49E9C19577}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247886" y="674146"/>
+          <a:ext cx="4643718" cy="2198594"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3624"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>PWR</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>190x100</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>235325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>26334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>198782</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="사각형: 둥근 모서리 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2600C0CC-B23E-468F-85E0-895EF1D5A717}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2948045" y="689274"/>
+          <a:ext cx="2934596" cy="2161268"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>CPU</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>120x100</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>107572</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>219246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>109403</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>11791</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="사각형: 둥근 모서리 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB6FD400-8A84-4FE9-A387-B86913778F37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3774137" y="3581011"/>
+          <a:ext cx="2422301" cy="4499015"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>48V SMPS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>203.1x101.6x40.6</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>197223</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="사각형: 둥근 모서리 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD919A1F-36AD-47BB-AD95-7C7018E672F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1017046" y="459890"/>
+          <a:ext cx="5062817" cy="9370807"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>157409</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>36638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>90036</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>175882</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="사각형: 둥근 모서리 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDB71F28-042C-421B-8C3B-5A8DFAC09788}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3823974" y="4518991"/>
+          <a:ext cx="2353097" cy="3501009"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>12V SMPS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>158x97x38</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>232635</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="사각형: 둥근 모서리 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031223A0-F521-446F-9EF3-769B7CCEBEBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1236682" y="8751793"/>
+          <a:ext cx="2432123" cy="661148"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>FAN</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80196</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>116347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>230354</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82728</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF583544-A03C-479F-91A0-E2E90AD394D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3524436" y="2547127"/>
+          <a:ext cx="881678" cy="187361"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>HD</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>78248</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>98614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>74544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F3937F5-50F5-4F5D-B8CB-1FA7DCA3327E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4497848" y="2529394"/>
+          <a:ext cx="575084" cy="196910"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>48V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12377</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>207066</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107673</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A9A120-06BF-4C82-8853-D55D98B83A4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5163497" y="2537773"/>
+          <a:ext cx="438529" cy="221660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>12V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>345842</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>168869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>522875</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>185531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="사각형: 둥근 모서리 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDAA6CF0-021C-4435-B830-64A1D4407458}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13192266" y="4427104"/>
+          <a:ext cx="965927" cy="4499015"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>48V SMPS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>203.1x101.6x40.6</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>89005</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>17835</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>376519</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>140025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="사각형: 둥근 모서리 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0794F4C8-86C1-4F43-8AE7-72F892B22D15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14396676" y="4500188"/>
+          <a:ext cx="959867" cy="3483955"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>12V SMPS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>158x97x38</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142726</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>183798</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>43962</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>148131</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B49F9732-3B51-4598-AB90-5646E4040F8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1392406" y="2614578"/>
+          <a:ext cx="632756" cy="185313"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DC48V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>234462</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>160957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>168331</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161637</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243666F5-BF95-447E-AF8E-C83491881238}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2459502" y="2591737"/>
+          <a:ext cx="421549" cy="221660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>12V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>82079</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166819</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>167499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB2106D-CD88-417F-A60F-5F80CFD6D420}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2063279" y="2597599"/>
+          <a:ext cx="352261" cy="221660"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>RF</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2049</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>153024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117357</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED878544-19D6-4C17-9697-DE3305B87584}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1251729" y="3909684"/>
+          <a:ext cx="638032" cy="185313"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DC48V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7345</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>40795</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>115765</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>41476</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23AD56CA-73D6-4212-9270-6AE0333494FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1744705" y="3355495"/>
+          <a:ext cx="352260" cy="221661"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>RF</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>159727</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>49587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>93596</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50268</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1E2D980-7A79-42A5-9FC7-B6800C44166C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2384767" y="3364287"/>
+          <a:ext cx="421549" cy="221661"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1200" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>12V</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>82924</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>233643</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="사각형: 둥근 모서리 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D952BF9-B7BE-4579-9806-5C2AB8714D33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7998759" y="466165"/>
+          <a:ext cx="4265519" cy="9502588"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>188259</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9354</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>181802</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="사각형: 둥근 모서리 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D2D80C-8313-4703-BBE0-B98D50058FAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10524565" y="681707"/>
+          <a:ext cx="49866" cy="2189507"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>CPU</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>120x100</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>238129</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>80684</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="사각형: 둥근 모서리 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEC6294D-63D5-4FA9-9A24-8D3077CB3C5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11784670" y="683559"/>
+          <a:ext cx="84602" cy="2229970"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3624"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+            <a:t>PWR</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>190x100</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>161363</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>27455</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>224117</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="사각형: 둥근 모서리 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95E0DE19-E6B6-4915-8121-61CBE6F60EF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10013575" y="528917"/>
+          <a:ext cx="2044515" cy="2608729"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>98613</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>205180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>233084</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>143436</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="사각형: 둥근 모서리 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26698AD-06DC-4EFA-A5F6-0E12971F3820}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10676966" y="877533"/>
+          <a:ext cx="1102659" cy="610609"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Heat </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>sink</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>224121</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="사각형: 둥근 모서리 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBB4D64-C2CE-4AED-BA88-A1F5E16765E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10578354" y="680310"/>
+          <a:ext cx="1192308" cy="126514"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>8965</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>233085</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="사각형: 둥근 모서리 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06714A05-17BF-4FEC-B7B6-C80E6EDB263E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10587318" y="2715298"/>
+          <a:ext cx="1192308" cy="126514"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>71718</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>97602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>179295</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>98610</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="사각형: 둥근 모서리 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E4D2C82-970D-4336-A997-EA0ED2CEDA8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10165977" y="1890543"/>
+          <a:ext cx="349624" cy="897479"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1"/>
+            <a:t>CPU</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>71718</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>43814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>179295</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="사각형: 둥근 모서리 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B8DED1-DEC6-48E6-9AE7-906E8C3B9196}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10165977" y="716167"/>
+          <a:ext cx="349624" cy="1103668"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1"/>
+            <a:t>FAN</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>143435</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>215153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>170403</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161608</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="34" name="그룹 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBABC761-D251-4943-BABB-1FFB140199F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="14451106" y="5818094"/>
+          <a:ext cx="2044026" cy="5325279"/>
+          <a:chOff x="8731550" y="452279"/>
+          <a:chExt cx="2088850" cy="4990223"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="사각형: 둥근 모서리 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FD9F962-0C5E-44B8-8411-DF2F5DB994B8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8731550" y="452279"/>
+            <a:ext cx="98125" cy="4990223"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 3334"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+              <a:t>RF</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>240x100</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="사각형: 둥근 모서리 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8D5B9EE-51E2-400E-AF77-2497A08E6FF6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8837998" y="1790699"/>
+            <a:ext cx="1982402" cy="2257425"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 1406"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+              <a:t>Heat</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+              <a:t>Sink</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>80x80x110</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="사각형: 둥근 모서리 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58CF4F39-2C09-44D8-90E5-2492EBF7B844}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8837998" y="1247775"/>
+            <a:ext cx="1982402" cy="533400"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 1406"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1"/>
+              <a:t>FAN</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1050" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>80x80x25</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>220880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>233081</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>167336</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="40" name="그룹 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EE9032E-0350-4648-ADED-3E96F7CCFAFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9699812" y="3582645"/>
+          <a:ext cx="2079810" cy="5325279"/>
+          <a:chOff x="9699812" y="3358527"/>
+          <a:chExt cx="2079810" cy="5325279"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="사각형: 둥근 모서리 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03F1CF37-F5B2-47FE-A153-8816C01CEA57}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="10776487" y="3358527"/>
+            <a:ext cx="52878" cy="5325279"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 3334"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+              <a:t>RF</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>240x100</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="사각형: 둥근 모서리 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E778B7C-6561-4ED9-A317-A3DDFE92C117}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="10065609" y="4266856"/>
+            <a:ext cx="701002" cy="1784319"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 1406"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Heat</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Sink</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="사각형: 둥근 모서리 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{093A682F-8DCC-4121-8A44-5B0F35C0F39A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="9699812" y="4270188"/>
+            <a:ext cx="367553" cy="1807884"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 1406"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>FAN</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="사각형: 둥근 모서리 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6455C44B-4F50-4D6F-9769-8DE2847961DE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10825467" y="4270026"/>
+            <a:ext cx="954155" cy="2623831"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 3334"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="2400" b="1"/>
+              <a:t>RF</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>240x100</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>8964</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>18490</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="사각형: 둥근 모서리 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735BB5C0-87CA-41EA-9CA4-DAA5FAE282D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9861176" y="3370729"/>
+          <a:ext cx="2187949" cy="5728447"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>8967</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="사각형: 둥근 모서리 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{209B8568-8B98-4997-8D41-E64E7A4B0B54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10847294" y="3593839"/>
+          <a:ext cx="1192308" cy="126514"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>8965</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>233085</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="사각형: 둥근 모서리 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9848033-02D1-4502-9C0B-4E95EACF8641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10829365" y="8784403"/>
+          <a:ext cx="1192308" cy="126514"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 1406"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1050" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9481,12 +12471,12 @@
       <c r="F4" s="24">
         <v>2</v>
       </c>
-      <c r="I4" s="64" t="s">
+      <c r="I4" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="73"/>
     </row>
     <row r="5" spans="4:20" x14ac:dyDescent="0.4">
       <c r="D5" s="6" t="s">
@@ -9625,12 +12615,12 @@
       <c r="L10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="61"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="49"/>
+      <c r="O10" s="68"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="56"/>
     </row>
     <row r="11" spans="4:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D11" s="9" t="s">
@@ -9654,14 +12644,14 @@
       <c r="L11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="58" t="s">
+      <c r="N11" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="O11" s="59"/>
-      <c r="S11" s="50" t="s">
+      <c r="O11" s="66"/>
+      <c r="S11" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="51"/>
+      <c r="T11" s="58"/>
     </row>
     <row r="12" spans="4:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D12" s="22" t="s">
@@ -9767,10 +12757,10 @@
       </c>
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.4">
-      <c r="I16" s="60" t="s">
+      <c r="I16" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="61"/>
+      <c r="J16" s="68"/>
       <c r="N16" s="16">
         <v>5</v>
       </c>
@@ -9781,10 +12771,10 @@
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="59"/>
+      <c r="J17" s="66"/>
       <c r="N17" s="6">
         <v>6</v>
       </c>
@@ -9840,32 +12830,32 @@
     </row>
     <row r="20" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="21" spans="9:20" x14ac:dyDescent="0.4">
-      <c r="I21" s="60" t="s">
+      <c r="I21" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="61"/>
-      <c r="N21" s="60" t="s">
+      <c r="J21" s="68"/>
+      <c r="N21" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="61"/>
-      <c r="S21" s="48" t="s">
+      <c r="O21" s="68"/>
+      <c r="S21" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="T21" s="49"/>
+      <c r="T21" s="56"/>
     </row>
     <row r="22" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I22" s="56" t="s">
+      <c r="I22" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="57"/>
-      <c r="N22" s="56" t="s">
+      <c r="J22" s="64"/>
+      <c r="N22" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="57"/>
-      <c r="S22" s="50" t="s">
+      <c r="O22" s="64"/>
+      <c r="S22" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="51"/>
+      <c r="T22" s="58"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I23" s="2">
@@ -9909,32 +12899,32 @@
     </row>
     <row r="25" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="26" spans="9:20" x14ac:dyDescent="0.4">
-      <c r="I26" s="60" t="s">
+      <c r="I26" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="61"/>
-      <c r="N26" s="60" t="s">
+      <c r="J26" s="68"/>
+      <c r="N26" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="O26" s="61"/>
-      <c r="S26" s="54" t="s">
+      <c r="O26" s="68"/>
+      <c r="S26" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="T26" s="55"/>
+      <c r="T26" s="62"/>
     </row>
     <row r="27" spans="9:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I27" s="58" t="s">
+      <c r="I27" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="59"/>
-      <c r="N27" s="58" t="s">
+      <c r="J27" s="66"/>
+      <c r="N27" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="59"/>
-      <c r="S27" s="52" t="s">
+      <c r="O27" s="66"/>
+      <c r="S27" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="T27" s="53"/>
+      <c r="T27" s="60"/>
     </row>
     <row r="28" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I28" s="2">
@@ -10038,40 +13028,40 @@
     </row>
     <row r="33" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="34" spans="9:23" x14ac:dyDescent="0.4">
-      <c r="I34" s="60" t="s">
+      <c r="I34" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="J34" s="61"/>
-      <c r="N34" s="60" t="s">
+      <c r="J34" s="68"/>
+      <c r="N34" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="O34" s="61"/>
-      <c r="S34" s="54" t="s">
+      <c r="O34" s="68"/>
+      <c r="S34" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="55"/>
-      <c r="V34" s="46" t="s">
+      <c r="T34" s="62"/>
+      <c r="V34" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="W34" s="47"/>
+      <c r="W34" s="54"/>
     </row>
     <row r="35" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I35" s="58" t="s">
+      <c r="I35" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="59"/>
-      <c r="N35" s="62" t="s">
+      <c r="J35" s="66"/>
+      <c r="N35" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="O35" s="63"/>
-      <c r="S35" s="56" t="s">
+      <c r="O35" s="70"/>
+      <c r="S35" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="T35" s="57"/>
-      <c r="V35" s="44" t="s">
+      <c r="T35" s="64"/>
+      <c r="V35" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="W35" s="45"/>
+      <c r="W35" s="52"/>
     </row>
     <row r="36" spans="9:23" x14ac:dyDescent="0.4">
       <c r="I36" s="2">
@@ -10172,10 +13162,10 @@
       </c>
     </row>
     <row r="40" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I40" s="60" t="s">
+      <c r="I40" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="J40" s="61"/>
+      <c r="J40" s="68"/>
       <c r="N40" s="9">
         <v>5</v>
       </c>
@@ -10196,10 +13186,10 @@
       </c>
     </row>
     <row r="41" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I41" s="58" t="s">
+      <c r="I41" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="59"/>
+      <c r="J41" s="66"/>
     </row>
     <row r="42" spans="9:23" x14ac:dyDescent="0.4">
       <c r="I42" s="2">
@@ -10208,10 +13198,10 @@
       <c r="J42" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N42" s="60" t="s">
+      <c r="N42" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="O42" s="61"/>
+      <c r="O42" s="68"/>
     </row>
     <row r="43" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I43" s="9">
@@ -10220,10 +13210,10 @@
       <c r="J43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N43" s="58" t="s">
+      <c r="N43" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="O43" s="59"/>
+      <c r="O43" s="66"/>
     </row>
     <row r="44" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="N44" s="2">
@@ -10234,10 +13224,10 @@
       </c>
     </row>
     <row r="45" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I45" s="60" t="s">
+      <c r="I45" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="61"/>
+      <c r="J45" s="68"/>
       <c r="N45" s="9">
         <v>2</v>
       </c>
@@ -10246,10 +13236,10 @@
       </c>
     </row>
     <row r="46" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I46" s="58" t="s">
+      <c r="I46" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="J46" s="59"/>
+      <c r="J46" s="66"/>
     </row>
     <row r="47" spans="9:23" x14ac:dyDescent="0.4">
       <c r="I47" s="2">
@@ -10258,10 +13248,10 @@
       <c r="J47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N47" s="60" t="s">
+      <c r="N47" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="O47" s="61"/>
+      <c r="O47" s="68"/>
     </row>
     <row r="48" spans="9:23" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I48" s="9">
@@ -10270,10 +13260,10 @@
       <c r="J48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N48" s="58" t="s">
+      <c r="N48" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="O48" s="59"/>
+      <c r="O48" s="66"/>
     </row>
     <row r="49" spans="11:15" x14ac:dyDescent="0.4">
       <c r="N49" s="2">
@@ -10348,7 +13338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
@@ -10431,38 +13421,38 @@
       <c r="D7" s="26">
         <v>5</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="61"/>
-      <c r="J7" s="60" t="s">
+      <c r="H7" s="68"/>
+      <c r="J7" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="61"/>
-      <c r="P7" s="60" t="s">
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="68"/>
+      <c r="P7" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="61"/>
-      <c r="U7" s="60" t="s">
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="68"/>
+      <c r="U7" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="V7" s="61"/>
-      <c r="Y7" s="72" t="s">
+      <c r="V7" s="68"/>
+      <c r="Y7" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="73"/>
-      <c r="AB7" s="54" t="s">
+      <c r="Z7" s="80"/>
+      <c r="AB7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AC7" s="55"/>
-      <c r="AF7" s="54" t="s">
+      <c r="AC7" s="62"/>
+      <c r="AF7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AG7" s="55"/>
+      <c r="AG7" s="62"/>
     </row>
     <row r="8" spans="2:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
@@ -10474,38 +13464,38 @@
       <c r="D8" s="26">
         <v>35</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="J8" s="67" t="s">
+      <c r="H8" s="64"/>
+      <c r="J8" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="68"/>
-      <c r="P8" s="67" t="s">
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="75"/>
+      <c r="P8" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="68"/>
-      <c r="U8" s="58" t="s">
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="75"/>
+      <c r="U8" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="V8" s="59"/>
-      <c r="Y8" s="70" t="s">
+      <c r="V8" s="66"/>
+      <c r="Y8" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="Z8" s="71"/>
-      <c r="AB8" s="56" t="s">
+      <c r="Z8" s="78"/>
+      <c r="AB8" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AC8" s="57"/>
-      <c r="AF8" s="56" t="s">
+      <c r="AC8" s="64"/>
+      <c r="AF8" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AG8" s="57"/>
+      <c r="AG8" s="64"/>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.4">
       <c r="B9" s="6" t="s">
@@ -10700,10 +13690,10 @@
         <f>SUM(D4:D11)</f>
         <v>150.19999999999999</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G12" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="61"/>
+      <c r="H12" s="68"/>
       <c r="J12" s="6">
         <v>7</v>
       </c>
@@ -10754,10 +13744,10 @@
       </c>
     </row>
     <row r="13" spans="2:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="59"/>
+      <c r="H13" s="66"/>
       <c r="J13" s="6">
         <v>9</v>
       </c>
@@ -10870,14 +13860,14 @@
       <c r="S15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="U15" s="60" t="s">
+      <c r="U15" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="V15" s="61"/>
-      <c r="Y15" s="60" t="s">
+      <c r="V15" s="68"/>
+      <c r="Y15" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="Z15" s="61"/>
+      <c r="Z15" s="68"/>
     </row>
     <row r="16" spans="2:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="G16" s="6">
@@ -10902,14 +13892,14 @@
         <v>16</v>
       </c>
       <c r="S16" s="8"/>
-      <c r="U16" s="58" t="s">
+      <c r="U16" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="V16" s="59"/>
-      <c r="Y16" s="58" t="s">
+      <c r="V16" s="66"/>
+      <c r="Y16" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="Z16" s="59"/>
+      <c r="Z16" s="66"/>
     </row>
     <row r="17" spans="7:29" x14ac:dyDescent="0.4">
       <c r="G17" s="6">
@@ -11001,40 +13991,40 @@
     </row>
     <row r="19" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="7:29" x14ac:dyDescent="0.4">
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="61"/>
-      <c r="L20" s="60" t="s">
+      <c r="H20" s="68"/>
+      <c r="L20" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="61"/>
-      <c r="U20" s="60" t="s">
+      <c r="M20" s="68"/>
+      <c r="U20" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="V20" s="61"/>
-      <c r="Y20" s="60" t="s">
+      <c r="V20" s="68"/>
+      <c r="Y20" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="Z20" s="61"/>
+      <c r="Z20" s="68"/>
     </row>
     <row r="21" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="59"/>
-      <c r="L21" s="58" t="s">
+      <c r="H21" s="66"/>
+      <c r="L21" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M21" s="59"/>
-      <c r="U21" s="58" t="s">
+      <c r="M21" s="66"/>
+      <c r="U21" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="V21" s="59"/>
-      <c r="Y21" s="58" t="s">
+      <c r="V21" s="66"/>
+      <c r="Y21" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="59"/>
+      <c r="Z21" s="66"/>
     </row>
     <row r="22" spans="7:29" x14ac:dyDescent="0.4">
       <c r="G22" s="2">
@@ -11109,10 +14099,10 @@
       </c>
     </row>
     <row r="25" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L25" s="60" t="s">
+      <c r="L25" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="61"/>
+      <c r="M25" s="68"/>
       <c r="U25" s="39">
         <v>4</v>
       </c>
@@ -11127,14 +14117,14 @@
       </c>
     </row>
     <row r="26" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G26" s="60" t="s">
+      <c r="G26" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="61"/>
-      <c r="L26" s="58" t="s">
+      <c r="H26" s="68"/>
+      <c r="L26" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="59"/>
+      <c r="M26" s="66"/>
       <c r="U26" s="42">
         <v>5</v>
       </c>
@@ -11149,10 +14139,10 @@
       </c>
     </row>
     <row r="27" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G27" s="58" t="s">
+      <c r="G27" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="59"/>
+      <c r="H27" s="66"/>
       <c r="L27" s="2">
         <v>1</v>
       </c>
@@ -11183,58 +14173,58 @@
       </c>
     </row>
     <row r="30" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L30" s="60" t="s">
+      <c r="L30" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="M30" s="61"/>
-      <c r="Y30" s="60" t="s">
+      <c r="M30" s="68"/>
+      <c r="Y30" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="Z30" s="61"/>
-      <c r="AB30" s="60" t="s">
+      <c r="Z30" s="68"/>
+      <c r="AB30" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="AC30" s="61"/>
+      <c r="AC30" s="68"/>
     </row>
     <row r="31" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G31" s="60" t="s">
+      <c r="G31" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="61"/>
-      <c r="L31" s="58" t="s">
+      <c r="H31" s="68"/>
+      <c r="L31" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="M31" s="59"/>
-      <c r="Y31" s="58" t="s">
+      <c r="M31" s="66"/>
+      <c r="Y31" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="Z31" s="59"/>
-      <c r="AB31" s="58" t="s">
+      <c r="Z31" s="66"/>
+      <c r="AB31" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AC31" s="59"/>
+      <c r="AC31" s="66"/>
     </row>
     <row r="32" spans="7:29" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G32" s="58" t="s">
+      <c r="G32" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="59"/>
-      <c r="L32" s="75">
+      <c r="H32" s="66"/>
+      <c r="L32" s="44">
         <v>1</v>
       </c>
-      <c r="M32" s="76" t="s">
+      <c r="M32" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="Y32" s="75">
+      <c r="Y32" s="44">
         <v>1</v>
       </c>
-      <c r="Z32" s="76" t="s">
+      <c r="Z32" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="AB32" s="75">
+      <c r="AB32" s="44">
         <v>1</v>
       </c>
-      <c r="AC32" s="76" t="s">
+      <c r="AC32" s="45" t="s">
         <v>95</v>
       </c>
     </row>
@@ -11245,22 +14235,22 @@
       <c r="H33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L33" s="77">
+      <c r="L33" s="46">
         <v>2</v>
       </c>
-      <c r="M33" s="78" t="s">
+      <c r="M33" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="Y33" s="77">
+      <c r="Y33" s="46">
         <v>2</v>
       </c>
-      <c r="Z33" s="78" t="s">
+      <c r="Z33" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AB33" s="79">
+      <c r="AB33" s="48">
         <v>2</v>
       </c>
-      <c r="AC33" s="80" t="s">
+      <c r="AC33" s="49" t="s">
         <v>96</v>
       </c>
     </row>
@@ -11271,48 +14261,48 @@
       <c r="H34" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="L34" s="79">
+      <c r="L34" s="48">
         <v>3</v>
       </c>
-      <c r="M34" s="80" t="s">
+      <c r="M34" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="Y34" s="79">
+      <c r="Y34" s="48">
         <v>3</v>
       </c>
-      <c r="Z34" s="80" t="s">
+      <c r="Z34" s="49" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="AF35" s="60" t="s">
+      <c r="AF35" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="AG35" s="61"/>
+      <c r="AG35" s="68"/>
     </row>
     <row r="36" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G36" s="60" t="s">
+      <c r="G36" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="H36" s="61"/>
-      <c r="L36" s="60" t="s">
+      <c r="H36" s="68"/>
+      <c r="L36" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="M36" s="61"/>
-      <c r="AF36" s="67" t="s">
+      <c r="M36" s="68"/>
+      <c r="AF36" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="AG36" s="68"/>
+      <c r="AG36" s="75"/>
     </row>
     <row r="37" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="G37" s="58" t="s">
+      <c r="G37" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="59"/>
-      <c r="L37" s="67" t="s">
+      <c r="H37" s="66"/>
+      <c r="L37" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="M37" s="68"/>
+      <c r="M37" s="75"/>
       <c r="AF37" s="2">
         <v>1</v>
       </c>
@@ -11355,26 +14345,26 @@
       </c>
     </row>
     <row r="40" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="AF40" s="60" t="s">
+      <c r="AF40" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="AG40" s="61"/>
+      <c r="AG40" s="68"/>
     </row>
     <row r="41" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L41" s="60" t="s">
+      <c r="L41" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="M41" s="61"/>
-      <c r="AF41" s="67" t="s">
+      <c r="M41" s="68"/>
+      <c r="AF41" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="AG41" s="68"/>
+      <c r="AG41" s="75"/>
     </row>
     <row r="42" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L42" s="67" t="s">
+      <c r="L42" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="M42" s="68"/>
+      <c r="M42" s="75"/>
       <c r="AF42" s="2">
         <v>1</v>
       </c>
@@ -11406,12 +14396,12 @@
     </row>
     <row r="45" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="46" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="J46" s="64" t="s">
+      <c r="J46" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="K46" s="65"/>
-      <c r="L46" s="65"/>
-      <c r="M46" s="66"/>
+      <c r="K46" s="72"/>
+      <c r="L46" s="72"/>
+      <c r="M46" s="73"/>
     </row>
     <row r="47" spans="7:33" x14ac:dyDescent="0.4">
       <c r="J47" s="2">
@@ -11426,10 +14416,10 @@
       <c r="M47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y47" s="60" t="s">
+      <c r="Y47" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="Z47" s="61"/>
+      <c r="Z47" s="68"/>
     </row>
     <row r="48" spans="7:33" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="J48" s="6">
@@ -11444,10 +14434,10 @@
       <c r="M48" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y48" s="67" t="s">
+      <c r="Y48" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="Z48" s="68"/>
+      <c r="Z48" s="75"/>
     </row>
     <row r="49" spans="10:26" x14ac:dyDescent="0.4">
       <c r="J49" s="6">
@@ -12392,10 +15382,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AT44"/>
+  <dimension ref="A1:AX44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AZ22" sqref="AZ22"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -12403,15 +15393,16 @@
     <col min="2" max="2" width="4.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="25" width="3.19921875" customWidth="1"/>
     <col min="28" max="28" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="56" width="3.19921875" customWidth="1"/>
+    <col min="29" max="47" width="3.19921875" customWidth="1"/>
+    <col min="48" max="48" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
       <c r="C2" s="34">
         <v>10</v>
       </c>
@@ -12537,7 +15528,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B3" s="33">
         <v>10</v>
       </c>
@@ -12545,23 +15536,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B4" s="33">
         <v>20</v>
       </c>
       <c r="AB4" s="33">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW4">
+        <v>45</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B5" s="33">
         <v>30</v>
       </c>
       <c r="AB5" s="33">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW5">
+        <v>50</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B6" s="33">
         <v>40</v>
       </c>
@@ -12569,23 +15578,35 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B7" s="33">
         <v>50</v>
       </c>
       <c r="AB7" s="33">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B8" s="33">
         <v>60</v>
       </c>
       <c r="AB8" s="33">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B9" s="33">
         <v>70</v>
       </c>
@@ -12598,61 +15619,110 @@
       <c r="AB9" s="33">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B10" s="33">
         <v>80</v>
       </c>
       <c r="AB10" s="33">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV10" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B11" s="33">
         <v>90</v>
       </c>
       <c r="AB11" s="33">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B12" s="33">
         <v>100</v>
       </c>
       <c r="AB12" s="33">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW12">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B13" s="33">
         <v>110</v>
       </c>
       <c r="AB13" s="33">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B14" s="33">
         <v>120</v>
       </c>
       <c r="AB14" s="33">
         <v>120</v>
       </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B15" s="33">
         <v>130</v>
       </c>
       <c r="AB15" s="33">
         <v>130</v>
       </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.4">
+      <c r="AV15" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
       <c r="B16" s="33">
         <v>140</v>
       </c>
       <c r="AB16" s="33">
         <v>140</v>
+      </c>
+      <c r="AV16" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW16" s="50">
+        <f>SUM(AW7:AW15)</f>
+        <v>94.199999999999989</v>
       </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.4">
@@ -12888,6 +15958,728 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0E493E-E73D-487A-B239-572961424B67}">
+  <dimension ref="A1:BC44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="25" width="3.19921875" customWidth="1"/>
+    <col min="28" max="45" width="3.19921875" customWidth="1"/>
+    <col min="46" max="46" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.19921875" customWidth="1"/>
+    <col min="48" max="48" width="10.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="C2" s="34">
+        <v>10</v>
+      </c>
+      <c r="D2" s="34">
+        <v>20</v>
+      </c>
+      <c r="E2" s="34">
+        <v>30</v>
+      </c>
+      <c r="F2" s="34">
+        <v>40</v>
+      </c>
+      <c r="G2" s="34">
+        <v>50</v>
+      </c>
+      <c r="H2" s="34">
+        <v>60</v>
+      </c>
+      <c r="I2" s="34">
+        <v>70</v>
+      </c>
+      <c r="J2" s="34">
+        <v>80</v>
+      </c>
+      <c r="K2" s="34">
+        <v>90</v>
+      </c>
+      <c r="L2" s="34">
+        <v>100</v>
+      </c>
+      <c r="M2" s="34">
+        <v>110</v>
+      </c>
+      <c r="N2" s="34">
+        <v>120</v>
+      </c>
+      <c r="O2" s="34">
+        <v>130</v>
+      </c>
+      <c r="P2" s="34">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="34">
+        <v>150</v>
+      </c>
+      <c r="R2" s="34">
+        <v>160</v>
+      </c>
+      <c r="S2" s="34">
+        <v>170</v>
+      </c>
+      <c r="T2" s="34">
+        <v>180</v>
+      </c>
+      <c r="U2" s="34">
+        <v>190</v>
+      </c>
+      <c r="V2" s="34">
+        <v>200</v>
+      </c>
+      <c r="W2" s="34">
+        <v>210</v>
+      </c>
+      <c r="X2" s="34">
+        <v>220</v>
+      </c>
+      <c r="Y2" s="34">
+        <v>230</v>
+      </c>
+      <c r="Z2" s="33"/>
+      <c r="AB2" s="34">
+        <v>180</v>
+      </c>
+      <c r="AC2" s="34">
+        <v>170</v>
+      </c>
+      <c r="AD2" s="34">
+        <v>160</v>
+      </c>
+      <c r="AE2" s="34">
+        <v>150</v>
+      </c>
+      <c r="AF2" s="34">
+        <v>140</v>
+      </c>
+      <c r="AG2" s="34">
+        <v>130</v>
+      </c>
+      <c r="AH2" s="34">
+        <v>120</v>
+      </c>
+      <c r="AI2" s="34">
+        <v>110</v>
+      </c>
+      <c r="AJ2" s="34">
+        <v>100</v>
+      </c>
+      <c r="AK2" s="34">
+        <v>90</v>
+      </c>
+      <c r="AL2" s="34">
+        <v>80</v>
+      </c>
+      <c r="AM2" s="34">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="34">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="34">
+        <v>50</v>
+      </c>
+      <c r="AP2" s="34">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="34">
+        <v>30</v>
+      </c>
+      <c r="AR2" s="34">
+        <v>20</v>
+      </c>
+      <c r="AS2" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B3" s="33">
+        <v>10</v>
+      </c>
+      <c r="AT3" s="33">
+        <v>10</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AW3">
+        <v>15</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ3">
+        <v>25</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B4" s="33">
+        <v>20</v>
+      </c>
+      <c r="AT4" s="33">
+        <v>20</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW4">
+        <v>45</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ4">
+        <v>30</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B5" s="33">
+        <v>30</v>
+      </c>
+      <c r="AT5" s="33">
+        <v>30</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW5">
+        <v>50</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B6" s="33">
+        <v>40</v>
+      </c>
+      <c r="AT6" s="33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B7" s="33">
+        <v>50</v>
+      </c>
+      <c r="AT7" s="33">
+        <v>50</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW7">
+        <v>3</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B8" s="33">
+        <v>60</v>
+      </c>
+      <c r="AT8" s="33">
+        <v>60</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW8">
+        <v>5</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ8">
+        <v>3</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B9" s="33">
+        <v>70</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT9" s="33">
+        <v>70</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW9">
+        <v>15</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ9">
+        <v>5</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B10" s="33">
+        <v>80</v>
+      </c>
+      <c r="AT10" s="33">
+        <v>80</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW10">
+        <v>1.6</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ10">
+        <v>80</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B11" s="33">
+        <v>90</v>
+      </c>
+      <c r="AT11" s="33">
+        <v>90</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW11">
+        <v>50</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ11">
+        <v>1.6</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>58</v>
+      </c>
+      <c r="BC11">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B12" s="33">
+        <v>100</v>
+      </c>
+      <c r="AT12" s="33">
+        <v>100</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW12">
+        <v>1.6</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AZ12">
+        <v>40</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>101</v>
+      </c>
+      <c r="BC12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B13" s="33">
+        <v>110</v>
+      </c>
+      <c r="AT13" s="33">
+        <v>110</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW13">
+        <v>10</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ13">
+        <v>10</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B14" s="33">
+        <v>120</v>
+      </c>
+      <c r="AT14" s="33">
+        <v>120</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW14">
+        <v>3</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ14">
+        <v>3</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B15" s="33">
+        <v>130</v>
+      </c>
+      <c r="AT15" s="33">
+        <v>130</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW15">
+        <v>5</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ15">
+        <v>5</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.4">
+      <c r="B16" s="33">
+        <v>140</v>
+      </c>
+      <c r="AT16" s="33">
+        <v>140</v>
+      </c>
+      <c r="AV16" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW16" s="50">
+        <f>SUM(AW7:AW15)</f>
+        <v>94.199999999999989</v>
+      </c>
+      <c r="AY16" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ16" s="50">
+        <f>SUM(AZ7:AZ15)</f>
+        <v>147.6</v>
+      </c>
+      <c r="BA16" s="50"/>
+      <c r="BB16" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC16" s="50">
+        <f>SUM(BC7:BC15)</f>
+        <v>122.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B17" s="33">
+        <v>150</v>
+      </c>
+      <c r="AT17" s="33">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B18" s="33">
+        <v>160</v>
+      </c>
+      <c r="AT18" s="33">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B19" s="33">
+        <v>170</v>
+      </c>
+      <c r="AT19" s="33">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B20" s="33">
+        <v>180</v>
+      </c>
+      <c r="AT20" s="33">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B21" s="33">
+        <v>190</v>
+      </c>
+      <c r="AT21" s="33">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B22" s="33">
+        <v>200</v>
+      </c>
+      <c r="AT22" s="33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B23" s="33">
+        <v>210</v>
+      </c>
+      <c r="AT23" s="33">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B24" s="33">
+        <v>220</v>
+      </c>
+      <c r="AT24" s="33">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B25" s="33">
+        <v>230</v>
+      </c>
+      <c r="AT25" s="33">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B26" s="33">
+        <v>240</v>
+      </c>
+      <c r="AT26" s="33">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B27" s="33">
+        <v>250</v>
+      </c>
+      <c r="AT27" s="33">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B28" s="33">
+        <v>260</v>
+      </c>
+      <c r="AT28" s="33">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B29" s="33">
+        <v>270</v>
+      </c>
+      <c r="AT29" s="33">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B30" s="33">
+        <v>280</v>
+      </c>
+      <c r="AT30" s="33">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="31" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B31" s="33">
+        <v>290</v>
+      </c>
+      <c r="AT31" s="33">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B32" s="33">
+        <v>300</v>
+      </c>
+      <c r="AT32" s="33">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B33" s="33">
+        <v>310</v>
+      </c>
+      <c r="AT33" s="33">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B34" s="33">
+        <v>320</v>
+      </c>
+      <c r="AT34" s="33">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B35" s="33">
+        <v>330</v>
+      </c>
+      <c r="AT35" s="33">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B36" s="33">
+        <v>340</v>
+      </c>
+      <c r="AT36" s="33">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B37" s="33">
+        <v>350</v>
+      </c>
+      <c r="AT37" s="33">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="38" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B38" s="33">
+        <v>360</v>
+      </c>
+      <c r="AT38" s="33">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B39" s="33">
+        <v>370</v>
+      </c>
+      <c r="AT39" s="33">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="40" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B40" s="33">
+        <v>380</v>
+      </c>
+      <c r="AT40" s="33">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B41" s="33">
+        <v>390</v>
+      </c>
+      <c r="AT41" s="33">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="42" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B42" s="33">
+        <v>400</v>
+      </c>
+      <c r="AT42" s="33">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B43" s="33">
+        <v>410</v>
+      </c>
+      <c r="AT43" s="33">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="2:46" x14ac:dyDescent="0.4">
+      <c r="B44" s="33">
+        <v>420</v>
+      </c>
+      <c r="AT44" s="33">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="D7:F10"/>
   <sheetViews>

</xml_diff>